<commit_message>
📊 Update Excel files from OneDrive - 2025-08-28 09:17:08
</commit_message>
<xml_diff>
--- a/backend/data/Spare_Parts_Inventory.xlsx
+++ b/backend/data/Spare_Parts_Inventory.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29225"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://vikramsolar0-my.sharepoint.com/personal/naveen_chamaria_vikramsolar_com/Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="5" documentId="8_{DFEF1166-70E6-421A-ABBC-F474D4E5088C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E2552D47-CD97-4BDB-A819-A1A0A24096F6}"/>
+  <xr:revisionPtr revIDLastSave="40" documentId="8_{DFEF1166-70E6-421A-ABBC-F474D4E5088C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F62D363E-96CC-496D-9853-5ABDDDF1D7A6}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{72449171-FCEF-49D6-AEAC-5AACDA2C6B26}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="82">
   <si>
     <t>Equipment_Category</t>
   </si>
@@ -77,12 +77,6 @@
     <t>HAIL_TESTER</t>
   </si>
   <si>
-    <t>H-001</t>
-  </si>
-  <si>
-    <t>HUASEN</t>
-  </si>
-  <si>
     <t>MLT_TESTER</t>
   </si>
   <si>
@@ -96,6 +90,198 @@
   </si>
   <si>
     <t>COMMON_PARTS</t>
+  </si>
+  <si>
+    <t>Bracket</t>
+  </si>
+  <si>
+    <t>Cylinder</t>
+  </si>
+  <si>
+    <t>CNC proportional valve</t>
+  </si>
+  <si>
+    <t>Pull pressure sensor</t>
+  </si>
+  <si>
+    <t>Sucker</t>
+  </si>
+  <si>
+    <t>Deformation sensor</t>
+  </si>
+  <si>
+    <t>Control cabinet system</t>
+  </si>
+  <si>
+    <t>PLC</t>
+  </si>
+  <si>
+    <t>IPC</t>
+  </si>
+  <si>
+    <t>Constant current power supply</t>
+  </si>
+  <si>
+    <t>Temperature sensor</t>
+  </si>
+  <si>
+    <t>Vacuum pump</t>
+  </si>
+  <si>
+    <t>Thermocouple</t>
+  </si>
+  <si>
+    <t>Deformation instrument</t>
+  </si>
+  <si>
+    <t>Tensimeter</t>
+  </si>
+  <si>
+    <t>Tension transmitter</t>
+  </si>
+  <si>
+    <t>Thermocouples</t>
+  </si>
+  <si>
+    <t>24V switching power supply</t>
+  </si>
+  <si>
+    <t>100V DC stabilized voltage power supply</t>
+  </si>
+  <si>
+    <t>Three color light indicator</t>
+  </si>
+  <si>
+    <t>Compressed air unit</t>
+  </si>
+  <si>
+    <t>Proportional valves</t>
+  </si>
+  <si>
+    <t>Five-way valves</t>
+  </si>
+  <si>
+    <t>Vacuum valves</t>
+  </si>
+  <si>
+    <t>Signal amplifiers</t>
+  </si>
+  <si>
+    <t>Support and mobile system</t>
+  </si>
+  <si>
+    <t>Ice ball gun head</t>
+  </si>
+  <si>
+    <t>Ice ball mold</t>
+  </si>
+  <si>
+    <t>Electronic balance</t>
+  </si>
+  <si>
+    <t>Vernier caliper</t>
+  </si>
+  <si>
+    <t>Ice ball freezer</t>
+  </si>
+  <si>
+    <t>Ice ball refrigerator</t>
+  </si>
+  <si>
+    <t>Control and acquisition system</t>
+  </si>
+  <si>
+    <t>Air tank</t>
+  </si>
+  <si>
+    <t>Valve</t>
+  </si>
+  <si>
+    <t>Gun</t>
+  </si>
+  <si>
+    <t>Speed sensor</t>
+  </si>
+  <si>
+    <t>Display screen</t>
+  </si>
+  <si>
+    <t>USB interface</t>
+  </si>
+  <si>
+    <t>Start button</t>
+  </si>
+  <si>
+    <t>Stop button</t>
+  </si>
+  <si>
+    <t>Emergency stop button</t>
+  </si>
+  <si>
+    <t>Power switch</t>
+  </si>
+  <si>
+    <t>Air switch</t>
+  </si>
+  <si>
+    <t>Drive motor</t>
+  </si>
+  <si>
+    <t>Counter</t>
+  </si>
+  <si>
+    <t>Φ12mm pipe</t>
+  </si>
+  <si>
+    <t>Compressed air source</t>
+  </si>
+  <si>
+    <t>Aviation plug</t>
+  </si>
+  <si>
+    <t>AC220V power supply</t>
+  </si>
+  <si>
+    <t>USB flash disk</t>
+  </si>
+  <si>
+    <t>Ice ball grinding tools</t>
+  </si>
+  <si>
+    <t>Waste ice ball treatment tank</t>
+  </si>
+  <si>
+    <t>Protective measures</t>
+  </si>
+  <si>
+    <t>Infrared ray system</t>
+  </si>
+  <si>
+    <t>Multiple fixtures</t>
+  </si>
+  <si>
+    <t>HEATER</t>
+  </si>
+  <si>
+    <t>4/6 mm2 Cu core cable</t>
+  </si>
+  <si>
+    <t>Flexible pvc piping</t>
+  </si>
+  <si>
+    <t>Led light for visual area</t>
+  </si>
+  <si>
+    <t>K type 4 channel data logger temperature/ thermal coupler</t>
+  </si>
+  <si>
+    <t>Temp and humidity data logger</t>
+  </si>
+  <si>
+    <t>Battery</t>
+  </si>
+  <si>
+    <t>Connector</t>
   </si>
 </sst>
 </file>
@@ -105,13 +291,25 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$-14009]yyyy\-mm\-dd;@"/>
   </numFmts>
-  <fonts count="1">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color indexed="8"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="10.5"/>
+      <color theme="1"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -140,10 +338,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -159,6 +361,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -478,25 +684,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{94C1C842-7533-49D8-BD7E-9BF474738299}">
-  <dimension ref="A1:L7"/>
+  <dimension ref="A1:L158"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+    <sheetView tabSelected="1" zoomScale="79" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.45"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="17.42578125" customWidth="1"/>
-    <col min="2" max="2" width="13.28515625" customWidth="1"/>
-    <col min="3" max="3" width="14.140625" customWidth="1"/>
-    <col min="4" max="4" width="17.5703125" customWidth="1"/>
-    <col min="5" max="5" width="21.42578125" customWidth="1"/>
-    <col min="6" max="6" width="16.5703125" customWidth="1"/>
-    <col min="7" max="7" width="17.5703125" customWidth="1"/>
-    <col min="8" max="8" width="11.85546875" customWidth="1"/>
-    <col min="9" max="9" width="16.42578125" customWidth="1"/>
-    <col min="10" max="10" width="20.85546875" customWidth="1"/>
-    <col min="11" max="11" width="19.85546875" style="2" customWidth="1"/>
+    <col min="1" max="1" width="22.81640625" customWidth="1"/>
+    <col min="2" max="2" width="53.7265625" customWidth="1"/>
+    <col min="3" max="3" width="14.1796875" customWidth="1"/>
+    <col min="4" max="4" width="17.54296875" customWidth="1"/>
+    <col min="5" max="5" width="21.453125" customWidth="1"/>
+    <col min="6" max="6" width="16.54296875" customWidth="1"/>
+    <col min="7" max="7" width="17.54296875" customWidth="1"/>
+    <col min="8" max="8" width="11.81640625" customWidth="1"/>
+    <col min="9" max="9" width="16.453125" customWidth="1"/>
+    <col min="10" max="10" width="20.81640625" customWidth="1"/>
+    <col min="11" max="11" width="19.81640625" style="2" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12">
@@ -539,59 +745,982 @@
     </row>
     <row r="2" spans="1:12">
       <c r="A2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C2">
-        <v>101</v>
-      </c>
-      <c r="D2">
-        <v>10000045210</v>
-      </c>
-      <c r="E2">
-        <v>1</v>
-      </c>
-      <c r="F2">
-        <v>3</v>
-      </c>
-      <c r="G2">
-        <v>5</v>
-      </c>
-      <c r="H2">
-        <v>2</v>
-      </c>
-      <c r="I2">
-        <v>35000</v>
-      </c>
-      <c r="J2" t="s">
-        <v>14</v>
+        <v>13</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="3" spans="1:12">
       <c r="A3" t="s">
-        <v>15</v>
+        <v>13</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="4" spans="1:12">
       <c r="A4" t="s">
-        <v>16</v>
+        <v>13</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="5" spans="1:12">
       <c r="A5" t="s">
-        <v>17</v>
+        <v>13</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="6" spans="1:12">
       <c r="A6" t="s">
-        <v>18</v>
+        <v>13</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="7" spans="1:12">
       <c r="A7" t="s">
-        <v>19</v>
+        <v>13</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12">
+      <c r="A8" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12">
+      <c r="A9" t="s">
+        <v>13</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12">
+      <c r="A10" t="s">
+        <v>13</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12">
+      <c r="A11" t="s">
+        <v>13</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12">
+      <c r="A12" t="s">
+        <v>13</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12">
+      <c r="A13" t="s">
+        <v>13</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12">
+      <c r="A14" t="s">
+        <v>13</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12">
+      <c r="A15" t="s">
+        <v>13</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12">
+      <c r="A16" t="s">
+        <v>13</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2">
+      <c r="A17" t="s">
+        <v>13</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2">
+      <c r="A18" t="s">
+        <v>13</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2">
+      <c r="A19" t="s">
+        <v>13</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2">
+      <c r="A20" t="s">
+        <v>13</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2">
+      <c r="A21" t="s">
+        <v>13</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2">
+      <c r="A22" t="s">
+        <v>13</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2">
+      <c r="A23" t="s">
+        <v>13</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2">
+      <c r="A24" t="s">
+        <v>13</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2">
+      <c r="A25" t="s">
+        <v>13</v>
+      </c>
+      <c r="B25" s="3" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2">
+      <c r="A26" t="s">
+        <v>13</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2">
+      <c r="A27" t="s">
+        <v>12</v>
+      </c>
+      <c r="B27" s="3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2">
+      <c r="A28" t="s">
+        <v>12</v>
+      </c>
+      <c r="B28" s="3" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2">
+      <c r="A29" t="s">
+        <v>12</v>
+      </c>
+      <c r="B29" s="3" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2">
+      <c r="A30" t="s">
+        <v>12</v>
+      </c>
+      <c r="B30" s="3" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2">
+      <c r="A31" t="s">
+        <v>12</v>
+      </c>
+      <c r="B31" s="3" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2">
+      <c r="A32" t="s">
+        <v>12</v>
+      </c>
+      <c r="B32" s="3" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2">
+      <c r="A33" t="s">
+        <v>12</v>
+      </c>
+      <c r="B33" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2">
+      <c r="A34" t="s">
+        <v>12</v>
+      </c>
+      <c r="B34" s="3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2">
+      <c r="A35" t="s">
+        <v>12</v>
+      </c>
+      <c r="B35" s="3" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2">
+      <c r="A36" t="s">
+        <v>12</v>
+      </c>
+      <c r="B36" s="3" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2">
+      <c r="A37" t="s">
+        <v>12</v>
+      </c>
+      <c r="B37" s="3" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2">
+      <c r="A38" t="s">
+        <v>12</v>
+      </c>
+      <c r="B38" s="3" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2">
+      <c r="A39" t="s">
+        <v>12</v>
+      </c>
+      <c r="B39" s="3" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2">
+      <c r="A40" t="s">
+        <v>12</v>
+      </c>
+      <c r="B40" s="3" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2">
+      <c r="A41" t="s">
+        <v>12</v>
+      </c>
+      <c r="B41" s="3" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2">
+      <c r="A42" t="s">
+        <v>12</v>
+      </c>
+      <c r="B42" s="3" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2">
+      <c r="A43" t="s">
+        <v>12</v>
+      </c>
+      <c r="B43" s="3" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2">
+      <c r="A44" t="s">
+        <v>12</v>
+      </c>
+      <c r="B44" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2">
+      <c r="A45" t="s">
+        <v>12</v>
+      </c>
+      <c r="B45" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2">
+      <c r="A46" t="s">
+        <v>12</v>
+      </c>
+      <c r="B46" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2">
+      <c r="A47" t="s">
+        <v>12</v>
+      </c>
+      <c r="B47" s="3" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2">
+      <c r="A48" t="s">
+        <v>12</v>
+      </c>
+      <c r="B48" s="3" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2">
+      <c r="A49" t="s">
+        <v>12</v>
+      </c>
+      <c r="B49" s="3" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2">
+      <c r="A50" t="s">
+        <v>12</v>
+      </c>
+      <c r="B50" s="3" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2">
+      <c r="A51" t="s">
+        <v>12</v>
+      </c>
+      <c r="B51" s="3" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2">
+      <c r="A52" t="s">
+        <v>12</v>
+      </c>
+      <c r="B52" s="3" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2">
+      <c r="A53" t="s">
+        <v>12</v>
+      </c>
+      <c r="B53" s="3" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2">
+      <c r="A54" t="s">
+        <v>12</v>
+      </c>
+      <c r="B54" s="3" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2">
+      <c r="A55" t="s">
+        <v>12</v>
+      </c>
+      <c r="B55" s="3" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2">
+      <c r="A56" t="s">
+        <v>12</v>
+      </c>
+      <c r="B56" s="3" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2">
+      <c r="A57" t="s">
+        <v>12</v>
+      </c>
+      <c r="B57" s="3" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2">
+      <c r="A58" t="s">
+        <v>12</v>
+      </c>
+      <c r="B58" s="3" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2">
+      <c r="A59" t="s">
+        <v>16</v>
+      </c>
+      <c r="B59" s="3" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" ht="17">
+      <c r="A60" t="s">
+        <v>17</v>
+      </c>
+      <c r="B60" s="4" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" ht="17">
+      <c r="A61" t="s">
+        <v>17</v>
+      </c>
+      <c r="B61" s="4" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" ht="17">
+      <c r="A62" t="s">
+        <v>17</v>
+      </c>
+      <c r="B62" s="4" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" ht="17">
+      <c r="A63" t="s">
+        <v>17</v>
+      </c>
+      <c r="B63" s="4" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" ht="17">
+      <c r="A64" t="s">
+        <v>17</v>
+      </c>
+      <c r="B64" s="4" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" ht="17">
+      <c r="A65" t="s">
+        <v>17</v>
+      </c>
+      <c r="B65" s="4" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" ht="17">
+      <c r="A66" t="s">
+        <v>17</v>
+      </c>
+      <c r="B66" s="4" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2">
+      <c r="A67" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2">
+      <c r="A68" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2">
+      <c r="A69" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2">
+      <c r="A70" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2">
+      <c r="A71" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2">
+      <c r="A72" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2">
+      <c r="A73" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2">
+      <c r="A74" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2">
+      <c r="A75" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2">
+      <c r="A76" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2">
+      <c r="A77" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2">
+      <c r="A78" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2">
+      <c r="A79" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2">
+      <c r="A80" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="81" spans="1:1">
+      <c r="A81" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="82" spans="1:1">
+      <c r="A82" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="83" spans="1:1">
+      <c r="A83" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="84" spans="1:1">
+      <c r="A84" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="85" spans="1:1">
+      <c r="A85" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="86" spans="1:1">
+      <c r="A86" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="87" spans="1:1">
+      <c r="A87" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="88" spans="1:1">
+      <c r="A88" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="89" spans="1:1">
+      <c r="A89" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="90" spans="1:1">
+      <c r="A90" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="91" spans="1:1">
+      <c r="A91" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="92" spans="1:1">
+      <c r="A92" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="93" spans="1:1">
+      <c r="A93" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="94" spans="1:1">
+      <c r="A94" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="95" spans="1:1">
+      <c r="A95" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="96" spans="1:1">
+      <c r="A96" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="97" spans="1:1">
+      <c r="A97" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="98" spans="1:1">
+      <c r="A98" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="99" spans="1:1">
+      <c r="A99" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="100" spans="1:1">
+      <c r="A100" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="101" spans="1:1">
+      <c r="A101" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="102" spans="1:1">
+      <c r="A102" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="103" spans="1:1">
+      <c r="A103" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="104" spans="1:1">
+      <c r="A104" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="105" spans="1:1">
+      <c r="A105" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="106" spans="1:1">
+      <c r="A106" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="107" spans="1:1">
+      <c r="A107" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="108" spans="1:1">
+      <c r="A108" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="109" spans="1:1">
+      <c r="A109" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="110" spans="1:1">
+      <c r="A110" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="111" spans="1:1">
+      <c r="A111" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="112" spans="1:1">
+      <c r="A112" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="113" spans="1:1">
+      <c r="A113" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="114" spans="1:1">
+      <c r="A114" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="115" spans="1:1">
+      <c r="A115" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="116" spans="1:1">
+      <c r="A116" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="117" spans="1:1">
+      <c r="A117" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="118" spans="1:1">
+      <c r="A118" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="119" spans="1:1">
+      <c r="A119" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="120" spans="1:1">
+      <c r="A120" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="121" spans="1:1">
+      <c r="A121" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="122" spans="1:1">
+      <c r="A122" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="123" spans="1:1">
+      <c r="A123" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="124" spans="1:1">
+      <c r="A124" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="125" spans="1:1">
+      <c r="A125" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="126" spans="1:1">
+      <c r="A126" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="127" spans="1:1">
+      <c r="A127" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="128" spans="1:1">
+      <c r="A128" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="129" spans="1:1">
+      <c r="A129" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="130" spans="1:1">
+      <c r="A130" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="131" spans="1:1">
+      <c r="A131" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="132" spans="1:1">
+      <c r="A132" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="133" spans="1:1">
+      <c r="A133" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="134" spans="1:1">
+      <c r="A134" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="135" spans="1:1">
+      <c r="A135" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="136" spans="1:1">
+      <c r="A136" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="137" spans="1:1">
+      <c r="A137" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="138" spans="1:1">
+      <c r="A138" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="139" spans="1:1">
+      <c r="A139" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="140" spans="1:1">
+      <c r="A140" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="141" spans="1:1">
+      <c r="A141" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="142" spans="1:1">
+      <c r="A142" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="143" spans="1:1">
+      <c r="A143" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="144" spans="1:1">
+      <c r="A144" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="145" spans="1:1">
+      <c r="A145" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="146" spans="1:1">
+      <c r="A146" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="147" spans="1:1">
+      <c r="A147" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="148" spans="1:1">
+      <c r="A148" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="149" spans="1:1">
+      <c r="A149" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="150" spans="1:1">
+      <c r="A150" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="151" spans="1:1">
+      <c r="A151" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="152" spans="1:1">
+      <c r="A152" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="153" spans="1:1">
+      <c r="A153" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="154" spans="1:1">
+      <c r="A154" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="155" spans="1:1">
+      <c r="A155" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="156" spans="1:1">
+      <c r="A156" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="157" spans="1:1">
+      <c r="A157" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="158" spans="1:1">
+      <c r="A158" t="s">
+        <v>15</v>
       </c>
     </row>
   </sheetData>
@@ -605,23 +1734,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="32f52b41-3b94-4090-a175-52d6bdf443eb" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100D4CAC9FC675B57408E93BF556641D4D2" ma:contentTypeVersion="12" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="274a8390434e2b99e5c0abfa3a3bc86a">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="32f52b41-3b94-4090-a175-52d6bdf443eb" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="396c0ffd131d9db66c00cc10498a82b8" ns3:_="">
     <xsd:import namespace="32f52b41-3b94-4090-a175-52d6bdf443eb"/>
@@ -815,14 +1927,61 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="32f52b41-3b94-4090-a175-52d6bdf443eb" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E0E37CA3-E383-451B-A722-9F0EA8A56E91}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{77BA3598-10A6-4EE4-9EA0-3517074D3A96}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="32f52b41-3b94-4090-a175-52d6bdf443eb"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5CE60954-2BCD-4F54-AE55-7D46BDC4758B}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5CE60954-2BCD-4F54-AE55-7D46BDC4758B}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{77BA3598-10A6-4EE4-9EA0-3517074D3A96}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E0E37CA3-E383-451B-A722-9F0EA8A56E91}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="32f52b41-3b94-4090-a175-52d6bdf443eb"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
📊 Update Excel files from OneDrive - 2025-08-29 09:42:06
</commit_message>
<xml_diff>
--- a/backend/data/Spare_Parts_Inventory.xlsx
+++ b/backend/data/Spare_Parts_Inventory.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://vikramsolar0-my.sharepoint.com/personal/naveen_chamaria_vikramsolar_com/Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="40" documentId="8_{DFEF1166-70E6-421A-ABBC-F474D4E5088C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F62D363E-96CC-496D-9853-5ABDDDF1D7A6}"/>
+  <xr:revisionPtr revIDLastSave="48" documentId="8_{DFEF1166-70E6-421A-ABBC-F474D4E5088C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F52CEF09-BEEF-4CB5-B41A-4A6AB4DF92D7}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{72449171-FCEF-49D6-AEAC-5AACDA2C6B26}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="86">
   <si>
     <t>Equipment_Category</t>
   </si>
@@ -282,6 +282,18 @@
   </si>
   <si>
     <t>Connector</t>
+  </si>
+  <si>
+    <t>Purlin</t>
+  </si>
+  <si>
+    <t>Clamps</t>
+  </si>
+  <si>
+    <t>M8-Bolts</t>
+  </si>
+  <si>
+    <t>Nuts</t>
   </si>
 </sst>
 </file>
@@ -684,10 +696,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{94C1C842-7533-49D8-BD7E-9BF474738299}">
-  <dimension ref="A1:L158"/>
+  <dimension ref="A1:L162"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="79" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -908,7 +920,7 @@
         <v>13</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>38</v>
+        <v>82</v>
       </c>
     </row>
     <row r="23" spans="1:2">
@@ -916,7 +928,7 @@
         <v>13</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>39</v>
+        <v>83</v>
       </c>
     </row>
     <row r="24" spans="1:2">
@@ -924,7 +936,7 @@
         <v>13</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>40</v>
+        <v>84</v>
       </c>
     </row>
     <row r="25" spans="1:2">
@@ -932,7 +944,7 @@
         <v>13</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>41</v>
+        <v>85</v>
       </c>
     </row>
     <row r="26" spans="1:2">
@@ -940,39 +952,39 @@
         <v>13</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
     </row>
     <row r="27" spans="1:2">
       <c r="A27" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
     </row>
     <row r="28" spans="1:2">
       <c r="A28" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
     </row>
     <row r="29" spans="1:2">
       <c r="A29" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
     </row>
     <row r="30" spans="1:2">
       <c r="A30" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
     </row>
     <row r="31" spans="1:2">
@@ -980,7 +992,7 @@
         <v>12</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
     </row>
     <row r="32" spans="1:2">
@@ -988,7 +1000,7 @@
         <v>12</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
     </row>
     <row r="33" spans="1:2">
@@ -996,7 +1008,7 @@
         <v>12</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
     </row>
     <row r="34" spans="1:2">
@@ -1004,7 +1016,7 @@
         <v>12</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
     </row>
     <row r="35" spans="1:2">
@@ -1012,7 +1024,7 @@
         <v>12</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
     </row>
     <row r="36" spans="1:2">
@@ -1020,7 +1032,7 @@
         <v>12</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
     </row>
     <row r="37" spans="1:2">
@@ -1028,7 +1040,7 @@
         <v>12</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
     </row>
     <row r="38" spans="1:2">
@@ -1036,7 +1048,7 @@
         <v>12</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
     </row>
     <row r="39" spans="1:2">
@@ -1044,7 +1056,7 @@
         <v>12</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
     </row>
     <row r="40" spans="1:2">
@@ -1052,7 +1064,7 @@
         <v>12</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
     </row>
     <row r="41" spans="1:2">
@@ -1060,7 +1072,7 @@
         <v>12</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
     </row>
     <row r="42" spans="1:2">
@@ -1068,7 +1080,7 @@
         <v>12</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
     </row>
     <row r="43" spans="1:2">
@@ -1076,7 +1088,7 @@
         <v>12</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
     </row>
     <row r="44" spans="1:2">
@@ -1084,7 +1096,7 @@
         <v>12</v>
       </c>
       <c r="B44" s="3" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
     </row>
     <row r="45" spans="1:2">
@@ -1092,7 +1104,7 @@
         <v>12</v>
       </c>
       <c r="B45" s="3" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
     </row>
     <row r="46" spans="1:2">
@@ -1100,7 +1112,7 @@
         <v>12</v>
       </c>
       <c r="B46" s="3" t="s">
-        <v>25</v>
+        <v>58</v>
       </c>
     </row>
     <row r="47" spans="1:2">
@@ -1108,7 +1120,7 @@
         <v>12</v>
       </c>
       <c r="B47" s="3" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
     </row>
     <row r="48" spans="1:2">
@@ -1116,7 +1128,7 @@
         <v>12</v>
       </c>
       <c r="B48" s="3" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
     </row>
     <row r="49" spans="1:2">
@@ -1124,7 +1136,7 @@
         <v>12</v>
       </c>
       <c r="B49" s="3" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
     </row>
     <row r="50" spans="1:2">
@@ -1132,7 +1144,7 @@
         <v>12</v>
       </c>
       <c r="B50" s="3" t="s">
-        <v>65</v>
+        <v>25</v>
       </c>
     </row>
     <row r="51" spans="1:2">
@@ -1140,7 +1152,7 @@
         <v>12</v>
       </c>
       <c r="B51" s="3" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
     </row>
     <row r="52" spans="1:2">
@@ -1148,7 +1160,7 @@
         <v>12</v>
       </c>
       <c r="B52" s="3" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
     </row>
     <row r="53" spans="1:2">
@@ -1156,7 +1168,7 @@
         <v>12</v>
       </c>
       <c r="B53" s="3" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
     </row>
     <row r="54" spans="1:2">
@@ -1164,7 +1176,7 @@
         <v>12</v>
       </c>
       <c r="B54" s="3" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
     </row>
     <row r="55" spans="1:2">
@@ -1172,7 +1184,7 @@
         <v>12</v>
       </c>
       <c r="B55" s="3" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
     </row>
     <row r="56" spans="1:2">
@@ -1180,7 +1192,7 @@
         <v>12</v>
       </c>
       <c r="B56" s="3" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
     </row>
     <row r="57" spans="1:2">
@@ -1188,7 +1200,7 @@
         <v>12</v>
       </c>
       <c r="B57" s="3" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
     </row>
     <row r="58" spans="1:2">
@@ -1196,47 +1208,47 @@
         <v>12</v>
       </c>
       <c r="B58" s="3" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
     </row>
     <row r="59" spans="1:2">
       <c r="A59" t="s">
+        <v>12</v>
+      </c>
+      <c r="B59" s="3" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2">
+      <c r="A60" t="s">
+        <v>12</v>
+      </c>
+      <c r="B60" s="3" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2">
+      <c r="A61" t="s">
+        <v>12</v>
+      </c>
+      <c r="B61" s="3" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2">
+      <c r="A62" t="s">
+        <v>12</v>
+      </c>
+      <c r="B62" s="3" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2">
+      <c r="A63" t="s">
         <v>16</v>
       </c>
-      <c r="B59" s="3" t="s">
+      <c r="B63" s="3" t="s">
         <v>74</v>
-      </c>
-    </row>
-    <row r="60" spans="1:2" ht="17">
-      <c r="A60" t="s">
-        <v>17</v>
-      </c>
-      <c r="B60" s="4" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="61" spans="1:2" ht="17">
-      <c r="A61" t="s">
-        <v>17</v>
-      </c>
-      <c r="B61" s="4" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="62" spans="1:2" ht="17">
-      <c r="A62" t="s">
-        <v>17</v>
-      </c>
-      <c r="B62" s="4" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="63" spans="1:2" ht="17">
-      <c r="A63" t="s">
-        <v>17</v>
-      </c>
-      <c r="B63" s="4" t="s">
-        <v>76</v>
       </c>
     </row>
     <row r="64" spans="1:2" ht="17">
@@ -1244,7 +1256,7 @@
         <v>17</v>
       </c>
       <c r="B64" s="4" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
     </row>
     <row r="65" spans="1:2" ht="17">
@@ -1252,7 +1264,7 @@
         <v>17</v>
       </c>
       <c r="B65" s="4" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
     </row>
     <row r="66" spans="1:2" ht="17">
@@ -1260,27 +1272,39 @@
         <v>17</v>
       </c>
       <c r="B66" s="4" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" ht="17">
+      <c r="A67" t="s">
+        <v>17</v>
+      </c>
+      <c r="B67" s="4" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" ht="17">
+      <c r="A68" t="s">
+        <v>17</v>
+      </c>
+      <c r="B68" s="4" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" ht="17">
+      <c r="A69" t="s">
+        <v>17</v>
+      </c>
+      <c r="B69" s="4" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" ht="17">
+      <c r="A70" t="s">
+        <v>17</v>
+      </c>
+      <c r="B70" s="4" t="s">
         <v>79</v>
-      </c>
-    </row>
-    <row r="67" spans="1:2">
-      <c r="A67" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="68" spans="1:2">
-      <c r="A68" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="69" spans="1:2">
-      <c r="A69" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="70" spans="1:2">
-      <c r="A70" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="71" spans="1:2">
@@ -1395,22 +1419,22 @@
     </row>
     <row r="93" spans="1:1">
       <c r="A93" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="94" spans="1:1">
       <c r="A94" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="95" spans="1:1">
       <c r="A95" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="96" spans="1:1">
       <c r="A96" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="97" spans="1:1">
@@ -1720,6 +1744,26 @@
     </row>
     <row r="158" spans="1:1">
       <c r="A158" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="159" spans="1:1">
+      <c r="A159" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="160" spans="1:1">
+      <c r="A160" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="161" spans="1:1">
+      <c r="A161" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="162" spans="1:1">
+      <c r="A162" t="s">
         <v>15</v>
       </c>
     </row>

</xml_diff>

<commit_message>
📊 Update Excel files from OneDrive - 2025-09-02 06:22:27
</commit_message>
<xml_diff>
--- a/backend/data/Spare_Parts_Inventory.xlsx
+++ b/backend/data/Spare_Parts_Inventory.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://vikramsolar0-my.sharepoint.com/personal/naveen_chamaria_vikramsolar_com/Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="48" documentId="8_{DFEF1166-70E6-421A-ABBC-F474D4E5088C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F52CEF09-BEEF-4CB5-B41A-4A6AB4DF92D7}"/>
+  <xr:revisionPtr revIDLastSave="112" documentId="8_{DFEF1166-70E6-421A-ABBC-F474D4E5088C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D9A1667A-C971-4DA1-BC4D-6376BACDC431}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{72449171-FCEF-49D6-AEAC-5AACDA2C6B26}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="628" uniqueCount="267">
   <si>
     <t>Equipment_Category</t>
   </si>
@@ -294,6 +294,549 @@
   </si>
   <si>
     <t>Nuts</t>
+  </si>
+  <si>
+    <t>ELCB (Earth Leakage Circuit Breaker)</t>
+  </si>
+  <si>
+    <t>MPCB (Motor Protection Circuit Breaker)</t>
+  </si>
+  <si>
+    <t>MCB (Miniature Circuit Breaker)</t>
+  </si>
+  <si>
+    <t>SPP (Single Phase Protection)</t>
+  </si>
+  <si>
+    <t>Industrial Socket and Plug Set</t>
+  </si>
+  <si>
+    <t>5mtrs Cable with Industrial Socket and Plug</t>
+  </si>
+  <si>
+    <t>Regulated Power Supply</t>
+  </si>
+  <si>
+    <t>Modular Controller</t>
+  </si>
+  <si>
+    <t>Contactors</t>
+  </si>
+  <si>
+    <t>PLC (Programmable Logic Control)</t>
+  </si>
+  <si>
+    <t>Relays</t>
+  </si>
+  <si>
+    <t>Thyrister</t>
+  </si>
+  <si>
+    <t>SSR's (Solid State Relay)</t>
+  </si>
+  <si>
+    <t>Transmitter</t>
+  </si>
+  <si>
+    <t>EMI Filter</t>
+  </si>
+  <si>
+    <t>Heater Contactor</t>
+  </si>
+  <si>
+    <t>Cool Relay</t>
+  </si>
+  <si>
+    <t>Inspection Lamp Relay</t>
+  </si>
+  <si>
+    <t>Thermal Fuse</t>
+  </si>
+  <si>
+    <t>8mm Push-in Type Connector</t>
+  </si>
+  <si>
+    <t>Stop Valve</t>
+  </si>
+  <si>
+    <t>BSP Screw Thread R 1/2" Connecting Sleeve Ø 12mm</t>
+  </si>
+  <si>
+    <t>Water Float Switch</t>
+  </si>
+  <si>
+    <t>Water Solenoid Valve</t>
+  </si>
+  <si>
+    <t>Water Inlet Solenoid Valve (for wick tank)</t>
+  </si>
+  <si>
+    <t>Compressor (Single Stage)</t>
+  </si>
+  <si>
+    <t>Oil Separator</t>
+  </si>
+  <si>
+    <t>Condenser</t>
+  </si>
+  <si>
+    <t>Filter-Drier</t>
+  </si>
+  <si>
+    <t>Sight Glass</t>
+  </si>
+  <si>
+    <t>Expansion Valve (TXV)</t>
+  </si>
+  <si>
+    <t>High Pressure Switch</t>
+  </si>
+  <si>
+    <t>Low Pressure Switch</t>
+  </si>
+  <si>
+    <t>Evaporator</t>
+  </si>
+  <si>
+    <t>Compressor Delay Timer</t>
+  </si>
+  <si>
+    <t>Hot Gas Solenoid Valve</t>
+  </si>
+  <si>
+    <t>Hot Gas Injection Valve</t>
+  </si>
+  <si>
+    <t>Liquid Bypass Solenoid Valve</t>
+  </si>
+  <si>
+    <t>Liquid Bypass Solenoid</t>
+  </si>
+  <si>
+    <t>Cool Solenoid Valve</t>
+  </si>
+  <si>
+    <t>Humidity Generator Solenoid</t>
+  </si>
+  <si>
+    <t>Compressor High Stage (HS)</t>
+  </si>
+  <si>
+    <t>Compressor Low Stage (LS)</t>
+  </si>
+  <si>
+    <t>Oil Separator HS</t>
+  </si>
+  <si>
+    <t>Oil Separator LS</t>
+  </si>
+  <si>
+    <t>Drier HS</t>
+  </si>
+  <si>
+    <t>Drier LS</t>
+  </si>
+  <si>
+    <t>Expansion Valve LS</t>
+  </si>
+  <si>
+    <t>Bypass Valve</t>
+  </si>
+  <si>
+    <t>Plate Heat Exchanger (BPHE)</t>
+  </si>
+  <si>
+    <t>Sight Glass HS</t>
+  </si>
+  <si>
+    <t>Stainless Steel Tubular Heaters</t>
+  </si>
+  <si>
+    <t>Immersion Heater</t>
+  </si>
+  <si>
+    <t>Humidity Generator Heater</t>
+  </si>
+  <si>
+    <t>Water Float Assembly</t>
+  </si>
+  <si>
+    <t>Over-temperature Cut-off Thermostat</t>
+  </si>
+  <si>
+    <t>RTD PT 100 Sensor (3mm diameter, 75mm length)</t>
+  </si>
+  <si>
+    <t>Capacitive Type Humidity Sensor</t>
+  </si>
+  <si>
+    <t>Safety Sensor (without red "O" Ring)</t>
+  </si>
+  <si>
+    <t>Dry-Bulb Sensor (with single red "O" Ring)</t>
+  </si>
+  <si>
+    <t>Pressure Sensors (High Stage)</t>
+  </si>
+  <si>
+    <t>Pressure Sensors (Low Stage)</t>
+  </si>
+  <si>
+    <t>Return Gas Temperature Sensors</t>
+  </si>
+  <si>
+    <t>Fan Motor (Air Circulation)</t>
+  </si>
+  <si>
+    <t>Fan Blades</t>
+  </si>
+  <si>
+    <t>Condenser Fan Motor</t>
+  </si>
+  <si>
+    <t>Condenser Fan Blades</t>
+  </si>
+  <si>
+    <t>Door Hinges</t>
+  </si>
+  <si>
+    <t>Door Lock/Latch Assembly</t>
+  </si>
+  <si>
+    <t>Door Limit Switch</t>
+  </si>
+  <si>
+    <t>Door Gaskets (Silicone, dual system)</t>
+  </si>
+  <si>
+    <t>Touch Screen Display (7" WVGA)</t>
+  </si>
+  <si>
+    <t>USB Port</t>
+  </si>
+  <si>
+    <t>Ethernet Port (RJ-45)</t>
+  </si>
+  <si>
+    <t>Inspection Lamp</t>
+  </si>
+  <si>
+    <t>Inspection Lamp Bulb</t>
+  </si>
+  <si>
+    <t>Defog Heater (for viewing window)</t>
+  </si>
+  <si>
+    <t>SMS Module (Optional)</t>
+  </si>
+  <si>
+    <t>Internal Memory/SD Card</t>
+  </si>
+  <si>
+    <t>Ethernet Cable</t>
+  </si>
+  <si>
+    <t>RJ45 Ethernet Cable</t>
+  </si>
+  <si>
+    <t>Gauge Manifold Set</t>
+  </si>
+  <si>
+    <t>USB Thumb Drive</t>
+  </si>
+  <si>
+    <t>Entry Port Plugs (Ø 125mm &amp; Ø 50mm)</t>
+  </si>
+  <si>
+    <t>Wick Cloth (for humidity sensors)</t>
+  </si>
+  <si>
+    <t>Nitrogen Cylinder</t>
+  </si>
+  <si>
+    <t>Brazing set with Oxy-Acetylene Cylinder</t>
+  </si>
+  <si>
+    <t>Vacuum Pump</t>
+  </si>
+  <si>
+    <t>Refrigerant (R-404A and R-23 for cascade systems)</t>
+  </si>
+  <si>
+    <t>Cleaning solvents and consumables</t>
+  </si>
+  <si>
+    <t>Main Switch/Breaker</t>
+  </si>
+  <si>
+    <t>Emergency Stop Switch</t>
+  </si>
+  <si>
+    <t>Phase Failure Relay</t>
+  </si>
+  <si>
+    <t>Voltage Monitor Relay</t>
+  </si>
+  <si>
+    <t>Enhanced Modular Controller</t>
+  </si>
+  <si>
+    <t>SIMATIC PLC (Programmable Logic Control)</t>
+  </si>
+  <si>
+    <t>Main Control Board</t>
+  </si>
+  <si>
+    <t>Power Supply Board</t>
+  </si>
+  <si>
+    <t>Communication Board</t>
+  </si>
+  <si>
+    <t>Main Contactor</t>
+  </si>
+  <si>
+    <t>Heater Contactors</t>
+  </si>
+  <si>
+    <t>Compressor Contactors (HS/LS)</t>
+  </si>
+  <si>
+    <t>Fan Motor Contactors</t>
+  </si>
+  <si>
+    <t>Auxiliary Relays</t>
+  </si>
+  <si>
+    <t>Thermal Overload Relays</t>
+  </si>
+  <si>
+    <t>SSR's (Solid State Relays)</t>
+  </si>
+  <si>
+    <t>Control Transformers</t>
+  </si>
+  <si>
+    <t>Indicator Lamps</t>
+  </si>
+  <si>
+    <t>Boiler Tank</t>
+  </si>
+  <si>
+    <t>DM Water Reservoir Tank</t>
+  </si>
+  <si>
+    <t>Water Solenoid Valve (boiler)</t>
+  </si>
+  <si>
+    <t>Water Solenoid Valve (wick tank)</t>
+  </si>
+  <si>
+    <t>Water Float Switch (boiler)</t>
+  </si>
+  <si>
+    <t>Water Float Switch (wick tank)</t>
+  </si>
+  <si>
+    <t>Water level adjuster float</t>
+  </si>
+  <si>
+    <t>Water Inlet Strainer</t>
+  </si>
+  <si>
+    <t>Wick Cup</t>
+  </si>
+  <si>
+    <t>High Stage (HS) Compressor</t>
+  </si>
+  <si>
+    <t>Low Stage (LS) Compressor</t>
+  </si>
+  <si>
+    <t>Compressor internal overload relay (HS)</t>
+  </si>
+  <si>
+    <t>Compressor internal overload relay (LS)</t>
+  </si>
+  <si>
+    <t>Compressor external HP/LP switch (HS)</t>
+  </si>
+  <si>
+    <t>Compressor external HP/LP switch (LS)</t>
+  </si>
+  <si>
+    <t>Condenser Fan</t>
+  </si>
+  <si>
+    <t>Filter-Drier HS</t>
+  </si>
+  <si>
+    <t>Filter-Drier LS</t>
+  </si>
+  <si>
+    <t>Sight Glass LS</t>
+  </si>
+  <si>
+    <t>Expansion Valve HS</t>
+  </si>
+  <si>
+    <t>Plate Heat Exchanger (BPHE/Cascade)</t>
+  </si>
+  <si>
+    <t>Hot Gas Bypass Valve</t>
+  </si>
+  <si>
+    <t>Liquid Bypass Valve</t>
+  </si>
+  <si>
+    <t>Air Heaters (Stainless Steel Tubular)</t>
+  </si>
+  <si>
+    <t>Defog Heater</t>
+  </si>
+  <si>
+    <t>Heater MCBs</t>
+  </si>
+  <si>
+    <t>SSRs for heaters</t>
+  </si>
+  <si>
+    <t>Thermostat</t>
+  </si>
+  <si>
+    <t>RTD PT100 Sensors (3mm dia, 75mm length)</t>
+  </si>
+  <si>
+    <t>Thermocouple sensors</t>
+  </si>
+  <si>
+    <t>Digital temperature sensors</t>
+  </si>
+  <si>
+    <t>Wet Bulb Sensor</t>
+  </si>
+  <si>
+    <t>HS Compressor SP (Suction Pressure) Sensor</t>
+  </si>
+  <si>
+    <t>HS Compressor DP (Discharge Pressure) Sensor</t>
+  </si>
+  <si>
+    <t>HS Compressor RGT (Return Gas Temperature) Sensor</t>
+  </si>
+  <si>
+    <t>LS Compressor SP Sensor</t>
+  </si>
+  <si>
+    <t>LS Compressor DP Sensor</t>
+  </si>
+  <si>
+    <t>LS Compressor RGT Sensor</t>
+  </si>
+  <si>
+    <t>Air Circulation Fan Blades</t>
+  </si>
+  <si>
+    <t>Chamber Gasket</t>
+  </si>
+  <si>
+    <t>Port Plugs (Ø 125mm &amp; Ø 50mm)</t>
+  </si>
+  <si>
+    <t>Thermal Insulation</t>
+  </si>
+  <si>
+    <t>Mounting Hardware</t>
+  </si>
+  <si>
+    <t>Bolts and Screws</t>
+  </si>
+  <si>
+    <t>7" WVGA LCD Color Touch Screen (800 x 480)</t>
+  </si>
+  <si>
+    <t>HMI Touch Screen Display</t>
+  </si>
+  <si>
+    <t>Screen Brightness Control</t>
+  </si>
+  <si>
+    <t>Touch Calibration System</t>
+  </si>
+  <si>
+    <t>USB Port (Type-A)</t>
+  </si>
+  <si>
+    <t>USB Port (Type-B)</t>
+  </si>
+  <si>
+    <t>USB Memory Interface</t>
+  </si>
+  <si>
+    <t>Lamp Delay Timer</t>
+  </si>
+  <si>
+    <t>Ethernet Communication Module</t>
+  </si>
+  <si>
+    <t>SMS Communication Module (Optional)</t>
+  </si>
+  <si>
+    <t>RS232/RS485 Ports</t>
+  </si>
+  <si>
+    <t>2GB SD Card</t>
+  </si>
+  <si>
+    <t>USB Cables (Type-A, Type-B)</t>
+  </si>
+  <si>
+    <t>Multiple Language Support</t>
+  </si>
+  <si>
+    <t>User Access Control System</t>
+  </si>
+  <si>
+    <t>Diagnostic Systems</t>
+  </si>
+  <si>
+    <t>R-404A (High Stage/Single Stage)</t>
+  </si>
+  <si>
+    <t>R-23 (Low Stage)</t>
+  </si>
+  <si>
+    <t>Manifold Gauge Set</t>
+  </si>
+  <si>
+    <t>Micron Gauge</t>
+  </si>
+  <si>
+    <t>Charging Scale</t>
+  </si>
+  <si>
+    <t>Leak Detection Equipment</t>
+  </si>
+  <si>
+    <t>Brazing Set with Oxy-Acetylene Cylinder</t>
+  </si>
+  <si>
+    <t>USB Thumb Drive (&lt;1.5GB)</t>
+  </si>
+  <si>
+    <t>Cleaning Solvents</t>
+  </si>
+  <si>
+    <t>Other Consumables</t>
+  </si>
+  <si>
+    <t>Control Panel Air Filter</t>
+  </si>
+  <si>
+    <t>Wire and Terminals</t>
+  </si>
+  <si>
+    <t>Loose Connection Supplies</t>
   </si>
 </sst>
 </file>
@@ -303,7 +846,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$-14009]yyyy\-mm\-dd;@"/>
   </numFmts>
-  <fonts count="3">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -322,6 +865,12 @@
       <color theme="1"/>
       <name val="Segoe UI"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color indexed="8"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
     </font>
   </fonts>
   <fills count="3">
@@ -350,14 +899,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -696,10 +1246,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{94C1C842-7533-49D8-BD7E-9BF474738299}">
-  <dimension ref="A1:L162"/>
+  <dimension ref="A1:L309"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="79" workbookViewId="0">
-      <selection activeCell="C27" sqref="C27"/>
+      <selection activeCell="A220" sqref="A220:XFD232"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -1307,464 +1857,1916 @@
         <v>79</v>
       </c>
     </row>
-    <row r="71" spans="1:2">
+    <row r="71" spans="1:2" ht="15.5">
       <c r="A71" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="72" spans="1:2">
+      <c r="B71" s="5" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" ht="15.5">
       <c r="A72" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="73" spans="1:2">
+      <c r="B72" s="5" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" ht="15.5">
       <c r="A73" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="74" spans="1:2">
+      <c r="B73" s="5" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" ht="15.5">
       <c r="A74" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="75" spans="1:2">
+      <c r="B74" s="5" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" ht="15.5">
       <c r="A75" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="76" spans="1:2">
+      <c r="B75" s="5" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" ht="15.5">
       <c r="A76" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="77" spans="1:2">
+      <c r="B76" s="5" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" ht="15.5">
       <c r="A77" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="78" spans="1:2">
+      <c r="B77" s="5" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" ht="15.5">
       <c r="A78" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="79" spans="1:2">
+      <c r="B78" s="5" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" ht="15.5">
       <c r="A79" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="80" spans="1:2">
+      <c r="B79" s="5" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2" ht="15.5">
       <c r="A80" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="81" spans="1:1">
+      <c r="B80" s="5" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" ht="15.5">
       <c r="A81" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="82" spans="1:1">
+      <c r="B81" s="5" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" ht="15.5">
       <c r="A82" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="83" spans="1:1">
+      <c r="B82" s="5" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" ht="15.5">
       <c r="A83" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="84" spans="1:1">
+      <c r="B83" s="5" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" ht="15.5">
       <c r="A84" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="85" spans="1:1">
+      <c r="B84" s="5" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" ht="15.5">
       <c r="A85" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="86" spans="1:1">
+      <c r="B85" s="5" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" ht="15.5">
       <c r="A86" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="87" spans="1:1">
+      <c r="B86" s="5" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2" ht="15.5">
       <c r="A87" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="88" spans="1:1">
+      <c r="B87" s="5" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2" ht="15.5">
       <c r="A88" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="89" spans="1:1">
+      <c r="B88" s="5" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2" ht="15.5">
       <c r="A89" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="90" spans="1:1">
+      <c r="B89" s="5" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2" ht="15.5">
       <c r="A90" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="91" spans="1:1">
+      <c r="B90" s="5" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2" ht="15.5">
       <c r="A91" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="92" spans="1:1">
+      <c r="B91" s="5" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2" ht="15.5">
       <c r="A92" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="93" spans="1:1">
+      <c r="B92" s="5" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2" ht="15.5">
       <c r="A93" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="94" spans="1:1">
+      <c r="B93" s="5" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2" ht="15.5">
       <c r="A94" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="95" spans="1:1">
+      <c r="B94" s="5" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2" ht="15.5">
       <c r="A95" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="96" spans="1:1">
+      <c r="B95" s="5" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2" ht="15.5">
       <c r="A96" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="97" spans="1:1">
+      <c r="B96" s="5" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2" ht="15.5">
       <c r="A97" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="98" spans="1:1">
+        <v>14</v>
+      </c>
+      <c r="B97" s="5" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2" ht="15.5">
       <c r="A98" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="99" spans="1:1">
+        <v>14</v>
+      </c>
+      <c r="B98" s="5" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2" ht="15.5">
       <c r="A99" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="100" spans="1:1">
+        <v>14</v>
+      </c>
+      <c r="B99" s="5" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2" ht="15.5">
       <c r="A100" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="101" spans="1:1">
+        <v>14</v>
+      </c>
+      <c r="B100" s="5" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2" ht="15.5">
       <c r="A101" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="102" spans="1:1">
+        <v>14</v>
+      </c>
+      <c r="B101" s="5" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="102" spans="1:2" ht="15.5">
       <c r="A102" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="103" spans="1:1">
+        <v>14</v>
+      </c>
+      <c r="B102" s="5" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="103" spans="1:2" ht="15.5">
       <c r="A103" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="104" spans="1:1">
+        <v>14</v>
+      </c>
+      <c r="B103" s="5" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="104" spans="1:2" ht="15.5">
       <c r="A104" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="105" spans="1:1">
+        <v>14</v>
+      </c>
+      <c r="B104" s="5" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="105" spans="1:2" ht="15.5">
       <c r="A105" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="106" spans="1:1">
+        <v>14</v>
+      </c>
+      <c r="B105" s="5" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="106" spans="1:2" ht="15.5">
       <c r="A106" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="107" spans="1:1">
+        <v>14</v>
+      </c>
+      <c r="B106" s="5" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="107" spans="1:2" ht="15.5">
       <c r="A107" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="108" spans="1:1">
+        <v>14</v>
+      </c>
+      <c r="B107" s="5" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="108" spans="1:2" ht="15.5">
       <c r="A108" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="109" spans="1:1">
+        <v>14</v>
+      </c>
+      <c r="B108" s="5" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="109" spans="1:2" ht="15.5">
       <c r="A109" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="110" spans="1:1">
+        <v>14</v>
+      </c>
+      <c r="B109" s="5" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="110" spans="1:2" ht="15.5">
       <c r="A110" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="111" spans="1:1">
+        <v>14</v>
+      </c>
+      <c r="B110" s="5" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="111" spans="1:2" ht="15.5">
       <c r="A111" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="112" spans="1:1">
+        <v>14</v>
+      </c>
+      <c r="B111" s="5" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="112" spans="1:2" ht="15.5">
       <c r="A112" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="113" spans="1:1">
+        <v>14</v>
+      </c>
+      <c r="B112" s="5" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="113" spans="1:2" ht="15.5">
       <c r="A113" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="114" spans="1:1">
+        <v>14</v>
+      </c>
+      <c r="B113" s="5" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="114" spans="1:2" ht="15.5">
       <c r="A114" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="115" spans="1:1">
+        <v>14</v>
+      </c>
+      <c r="B114" s="5" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="115" spans="1:2" ht="15.5">
       <c r="A115" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="116" spans="1:1">
+        <v>14</v>
+      </c>
+      <c r="B115" s="5" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="116" spans="1:2" ht="15.5">
       <c r="A116" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="117" spans="1:1">
+        <v>14</v>
+      </c>
+      <c r="B116" s="5" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="117" spans="1:2" ht="15.5">
       <c r="A117" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="118" spans="1:1">
+        <v>14</v>
+      </c>
+      <c r="B117" s="5" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="118" spans="1:2" ht="15.5">
       <c r="A118" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="119" spans="1:1">
+        <v>14</v>
+      </c>
+      <c r="B118" s="5" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="119" spans="1:2" ht="15.5">
       <c r="A119" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="120" spans="1:1">
+        <v>14</v>
+      </c>
+      <c r="B119" s="5" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="120" spans="1:2" ht="15.5">
       <c r="A120" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="121" spans="1:1">
+        <v>14</v>
+      </c>
+      <c r="B120" s="5" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="121" spans="1:2" ht="15.5">
       <c r="A121" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="122" spans="1:1">
+        <v>14</v>
+      </c>
+      <c r="B121" s="5" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="122" spans="1:2" ht="15.5">
       <c r="A122" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="123" spans="1:1">
+        <v>14</v>
+      </c>
+      <c r="B122" s="5" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="123" spans="1:2" ht="15.5">
       <c r="A123" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="124" spans="1:1">
+        <v>14</v>
+      </c>
+      <c r="B123" s="5" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="124" spans="1:2" ht="15.5">
       <c r="A124" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="125" spans="1:1">
+        <v>14</v>
+      </c>
+      <c r="B124" s="5" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="125" spans="1:2" ht="15.5">
       <c r="A125" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="126" spans="1:1">
+        <v>14</v>
+      </c>
+      <c r="B125" s="5" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="126" spans="1:2" ht="15.5">
       <c r="A126" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="127" spans="1:1">
+        <v>14</v>
+      </c>
+      <c r="B126" s="5" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="127" spans="1:2" ht="15.5">
       <c r="A127" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="128" spans="1:1">
+        <v>14</v>
+      </c>
+      <c r="B127" s="5" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="128" spans="1:2" ht="15.5">
       <c r="A128" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="129" spans="1:1">
+        <v>14</v>
+      </c>
+      <c r="B128" s="5" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="129" spans="1:2" ht="15.5">
       <c r="A129" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="130" spans="1:1">
+        <v>14</v>
+      </c>
+      <c r="B129" s="5" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="130" spans="1:2" ht="15.5">
       <c r="A130" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="131" spans="1:1">
+        <v>14</v>
+      </c>
+      <c r="B130" s="5" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="131" spans="1:2" ht="15.5">
       <c r="A131" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="132" spans="1:1">
+        <v>14</v>
+      </c>
+      <c r="B131" s="5" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="132" spans="1:2" ht="15.5">
       <c r="A132" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="133" spans="1:1">
+        <v>14</v>
+      </c>
+      <c r="B132" s="5" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="133" spans="1:2" ht="15.5">
       <c r="A133" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="134" spans="1:1">
+        <v>14</v>
+      </c>
+      <c r="B133" s="5" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="134" spans="1:2" ht="15.5">
       <c r="A134" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="135" spans="1:1">
+        <v>14</v>
+      </c>
+      <c r="B134" s="5" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="135" spans="1:2" ht="15.5">
       <c r="A135" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="136" spans="1:1">
+        <v>14</v>
+      </c>
+      <c r="B135" s="5" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="136" spans="1:2" ht="15.5">
       <c r="A136" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="137" spans="1:1">
+        <v>14</v>
+      </c>
+      <c r="B136" s="5" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="137" spans="1:2" ht="15.5">
       <c r="A137" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="138" spans="1:1">
+        <v>14</v>
+      </c>
+      <c r="B137" s="5" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="138" spans="1:2" ht="15.5">
       <c r="A138" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="139" spans="1:1">
+        <v>14</v>
+      </c>
+      <c r="B138" s="5" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="139" spans="1:2" ht="15.5">
       <c r="A139" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="140" spans="1:1">
+        <v>14</v>
+      </c>
+      <c r="B139" s="5" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="140" spans="1:2" ht="15.5">
       <c r="A140" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="141" spans="1:1">
+        <v>14</v>
+      </c>
+      <c r="B140" s="5" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="141" spans="1:2" ht="15.5">
       <c r="A141" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="142" spans="1:1">
+        <v>14</v>
+      </c>
+      <c r="B141" s="5" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="142" spans="1:2" ht="15.5">
       <c r="A142" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="143" spans="1:1">
+        <v>14</v>
+      </c>
+      <c r="B142" s="5" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="143" spans="1:2" ht="15.5">
       <c r="A143" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="144" spans="1:1">
+        <v>14</v>
+      </c>
+      <c r="B143" s="5" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="144" spans="1:2" ht="15.5">
       <c r="A144" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="145" spans="1:1">
+        <v>14</v>
+      </c>
+      <c r="B144" s="5" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="145" spans="1:2" ht="15.5">
       <c r="A145" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="146" spans="1:1">
+        <v>14</v>
+      </c>
+      <c r="B145" s="5" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="146" spans="1:2" ht="15.5">
       <c r="A146" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="147" spans="1:1">
+        <v>14</v>
+      </c>
+      <c r="B146" s="5" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="147" spans="1:2" ht="15.5">
       <c r="A147" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="148" spans="1:1">
+        <v>14</v>
+      </c>
+      <c r="B147" s="5" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="148" spans="1:2" ht="15.5">
       <c r="A148" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="149" spans="1:1">
+        <v>14</v>
+      </c>
+      <c r="B148" s="5" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="149" spans="1:2" ht="15.5">
       <c r="A149" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="150" spans="1:1">
+        <v>14</v>
+      </c>
+      <c r="B149" s="5" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="150" spans="1:2" ht="15.5">
       <c r="A150" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="151" spans="1:1">
+        <v>14</v>
+      </c>
+      <c r="B150" s="5" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="151" spans="1:2" ht="15.5">
       <c r="A151" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="152" spans="1:1">
+        <v>14</v>
+      </c>
+      <c r="B151" s="5" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="152" spans="1:2" ht="15.5">
       <c r="A152" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="153" spans="1:1">
+        <v>14</v>
+      </c>
+      <c r="B152" s="5" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="153" spans="1:2" ht="15.5">
       <c r="A153" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="154" spans="1:1">
+        <v>14</v>
+      </c>
+      <c r="B153" s="5" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="154" spans="1:2" ht="15.5">
       <c r="A154" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="155" spans="1:1">
+        <v>14</v>
+      </c>
+      <c r="B154" s="5" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="155" spans="1:2" ht="15.5">
       <c r="A155" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="156" spans="1:1">
+        <v>14</v>
+      </c>
+      <c r="B155" s="5" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="156" spans="1:2" ht="15.5">
       <c r="A156" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="157" spans="1:1">
+        <v>14</v>
+      </c>
+      <c r="B156" s="5" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="157" spans="1:2" ht="15.5">
       <c r="A157" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="158" spans="1:1">
+        <v>14</v>
+      </c>
+      <c r="B157" s="5" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="158" spans="1:2" ht="15.5">
       <c r="A158" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="159" spans="1:1">
+        <v>14</v>
+      </c>
+      <c r="B158" s="5" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="159" spans="1:2" ht="15.5">
       <c r="A159" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="160" spans="1:1">
+        <v>14</v>
+      </c>
+      <c r="B159" s="5" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="160" spans="1:2" ht="15.5">
       <c r="A160" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="161" spans="1:1">
+        <v>14</v>
+      </c>
+      <c r="B160" s="5" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="161" spans="1:2" ht="15.5">
       <c r="A161" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="162" spans="1:1">
+        <v>14</v>
+      </c>
+      <c r="B161" s="5" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="162" spans="1:2" ht="15.5">
       <c r="A162" t="s">
-        <v>15</v>
+        <v>14</v>
+      </c>
+      <c r="B162" s="5" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="163" spans="1:2" ht="15.5">
+      <c r="A163" t="s">
+        <v>14</v>
+      </c>
+      <c r="B163" s="5" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="164" spans="1:2" ht="15.5">
+      <c r="A164" t="s">
+        <v>14</v>
+      </c>
+      <c r="B164" s="5" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="165" spans="1:2" ht="15.5">
+      <c r="A165" t="s">
+        <v>14</v>
+      </c>
+      <c r="B165" s="5" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="166" spans="1:2" ht="15.5">
+      <c r="A166" t="s">
+        <v>14</v>
+      </c>
+      <c r="B166" s="5" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="167" spans="1:2" ht="15.5">
+      <c r="A167" t="s">
+        <v>14</v>
+      </c>
+      <c r="B167" s="5" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="168" spans="1:2" ht="15.5">
+      <c r="A168" t="s">
+        <v>14</v>
+      </c>
+      <c r="B168" s="5" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="169" spans="1:2" ht="15.5">
+      <c r="A169" t="s">
+        <v>14</v>
+      </c>
+      <c r="B169" s="5" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="170" spans="1:2" ht="15.5">
+      <c r="A170" t="s">
+        <v>14</v>
+      </c>
+      <c r="B170" s="5" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="171" spans="1:2" ht="15.5">
+      <c r="A171" t="s">
+        <v>14</v>
+      </c>
+      <c r="B171" s="5" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="172" spans="1:2" ht="15.5">
+      <c r="A172" t="s">
+        <v>14</v>
+      </c>
+      <c r="B172" s="5" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="173" spans="1:2" ht="15.5">
+      <c r="A173" t="s">
+        <v>14</v>
+      </c>
+      <c r="B173" s="5" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="174" spans="1:2" ht="15.5">
+      <c r="A174" t="s">
+        <v>14</v>
+      </c>
+      <c r="B174" s="5" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="175" spans="1:2" ht="15.5">
+      <c r="A175" t="s">
+        <v>14</v>
+      </c>
+      <c r="B175" s="5" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="176" spans="1:2" ht="15.5">
+      <c r="A176" t="s">
+        <v>14</v>
+      </c>
+      <c r="B176" s="5" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="177" spans="1:2" ht="15.5">
+      <c r="A177" t="s">
+        <v>14</v>
+      </c>
+      <c r="B177" s="5" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="178" spans="1:2" ht="15.5">
+      <c r="A178" t="s">
+        <v>14</v>
+      </c>
+      <c r="B178" s="5" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="179" spans="1:2" ht="15.5">
+      <c r="A179" t="s">
+        <v>14</v>
+      </c>
+      <c r="B179" s="5" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="180" spans="1:2" ht="15.5">
+      <c r="A180" t="s">
+        <v>14</v>
+      </c>
+      <c r="B180" s="5" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="181" spans="1:2" ht="15.5">
+      <c r="A181" t="s">
+        <v>14</v>
+      </c>
+      <c r="B181" s="5" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="182" spans="1:2" ht="15.5">
+      <c r="A182" t="s">
+        <v>14</v>
+      </c>
+      <c r="B182" s="5" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="183" spans="1:2" ht="15.5">
+      <c r="A183" t="s">
+        <v>14</v>
+      </c>
+      <c r="B183" s="5" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="184" spans="1:2" ht="15.5">
+      <c r="A184" t="s">
+        <v>14</v>
+      </c>
+      <c r="B184" s="5" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="185" spans="1:2" ht="15.5">
+      <c r="A185" t="s">
+        <v>14</v>
+      </c>
+      <c r="B185" s="5" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="186" spans="1:2" ht="15.5">
+      <c r="A186" t="s">
+        <v>14</v>
+      </c>
+      <c r="B186" s="5" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="187" spans="1:2" ht="15.5">
+      <c r="A187" t="s">
+        <v>14</v>
+      </c>
+      <c r="B187" s="5" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="188" spans="1:2" ht="15.5">
+      <c r="A188" t="s">
+        <v>14</v>
+      </c>
+      <c r="B188" s="5" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="189" spans="1:2" ht="15.5">
+      <c r="A189" t="s">
+        <v>14</v>
+      </c>
+      <c r="B189" s="5" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="190" spans="1:2" ht="15.5">
+      <c r="A190" t="s">
+        <v>14</v>
+      </c>
+      <c r="B190" s="5" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="191" spans="1:2" ht="15.5">
+      <c r="A191" t="s">
+        <v>14</v>
+      </c>
+      <c r="B191" s="5" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="192" spans="1:2" ht="15.5">
+      <c r="A192" t="s">
+        <v>14</v>
+      </c>
+      <c r="B192" s="5" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="193" spans="1:2" ht="15.5">
+      <c r="A193" t="s">
+        <v>14</v>
+      </c>
+      <c r="B193" s="5" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="194" spans="1:2" ht="15.5">
+      <c r="A194" t="s">
+        <v>14</v>
+      </c>
+      <c r="B194" s="5" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="195" spans="1:2" ht="15.5">
+      <c r="A195" t="s">
+        <v>14</v>
+      </c>
+      <c r="B195" s="5" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="196" spans="1:2" ht="15.5">
+      <c r="A196" t="s">
+        <v>14</v>
+      </c>
+      <c r="B196" s="5" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="197" spans="1:2" ht="15.5">
+      <c r="A197" t="s">
+        <v>14</v>
+      </c>
+      <c r="B197" s="5" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="198" spans="1:2" ht="15.5">
+      <c r="A198" t="s">
+        <v>14</v>
+      </c>
+      <c r="B198" s="5" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="199" spans="1:2" ht="15.5">
+      <c r="A199" t="s">
+        <v>14</v>
+      </c>
+      <c r="B199" s="5" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="200" spans="1:2" ht="15.5">
+      <c r="A200" t="s">
+        <v>14</v>
+      </c>
+      <c r="B200" s="5" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="201" spans="1:2" ht="15.5">
+      <c r="A201" t="s">
+        <v>14</v>
+      </c>
+      <c r="B201" s="5" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="202" spans="1:2" ht="15.5">
+      <c r="A202" t="s">
+        <v>14</v>
+      </c>
+      <c r="B202" s="5" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="203" spans="1:2" ht="15.5">
+      <c r="A203" t="s">
+        <v>14</v>
+      </c>
+      <c r="B203" s="5" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="204" spans="1:2" ht="15.5">
+      <c r="A204" t="s">
+        <v>14</v>
+      </c>
+      <c r="B204" s="5" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="205" spans="1:2" ht="15.5">
+      <c r="A205" t="s">
+        <v>14</v>
+      </c>
+      <c r="B205" s="5" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="206" spans="1:2" ht="15.5">
+      <c r="A206" t="s">
+        <v>14</v>
+      </c>
+      <c r="B206" s="5" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="207" spans="1:2" ht="15.5">
+      <c r="A207" t="s">
+        <v>14</v>
+      </c>
+      <c r="B207" s="5" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="208" spans="1:2" ht="15.5">
+      <c r="A208" t="s">
+        <v>14</v>
+      </c>
+      <c r="B208" s="5" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="209" spans="1:2" ht="15.5">
+      <c r="A209" t="s">
+        <v>14</v>
+      </c>
+      <c r="B209" s="5" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="210" spans="1:2" ht="15.5">
+      <c r="A210" t="s">
+        <v>14</v>
+      </c>
+      <c r="B210" s="5" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="211" spans="1:2" ht="15.5">
+      <c r="A211" t="s">
+        <v>14</v>
+      </c>
+      <c r="B211" s="5" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="212" spans="1:2" ht="15.5">
+      <c r="A212" t="s">
+        <v>14</v>
+      </c>
+      <c r="B212" s="5" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="213" spans="1:2" ht="15.5">
+      <c r="A213" t="s">
+        <v>14</v>
+      </c>
+      <c r="B213" s="5" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="214" spans="1:2" ht="15.5">
+      <c r="A214" t="s">
+        <v>14</v>
+      </c>
+      <c r="B214" s="5" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="215" spans="1:2" ht="15.5">
+      <c r="A215" t="s">
+        <v>14</v>
+      </c>
+      <c r="B215" s="5" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="216" spans="1:2" ht="15.5">
+      <c r="A216" t="s">
+        <v>14</v>
+      </c>
+      <c r="B216" s="5" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="217" spans="1:2" ht="15.5">
+      <c r="A217" t="s">
+        <v>14</v>
+      </c>
+      <c r="B217" s="5" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="218" spans="1:2" ht="15.5">
+      <c r="A218" t="s">
+        <v>14</v>
+      </c>
+      <c r="B218" s="5" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="219" spans="1:2" ht="15.5">
+      <c r="A219" t="s">
+        <v>14</v>
+      </c>
+      <c r="B219" s="5" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="220" spans="1:2" ht="15.5">
+      <c r="A220" t="s">
+        <v>15</v>
+      </c>
+      <c r="B220" s="5" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="221" spans="1:2" ht="15.5">
+      <c r="A221" t="s">
+        <v>15</v>
+      </c>
+      <c r="B221" s="5" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="222" spans="1:2" ht="15.5">
+      <c r="A222" t="s">
+        <v>15</v>
+      </c>
+      <c r="B222" s="5" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="223" spans="1:2" ht="15.5">
+      <c r="A223" t="s">
+        <v>15</v>
+      </c>
+      <c r="B223" s="5" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="224" spans="1:2" ht="15.5">
+      <c r="A224" t="s">
+        <v>15</v>
+      </c>
+      <c r="B224" s="5" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="225" spans="1:2" ht="15.5">
+      <c r="A225" t="s">
+        <v>15</v>
+      </c>
+      <c r="B225" s="5" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="226" spans="1:2" ht="15.5">
+      <c r="A226" t="s">
+        <v>15</v>
+      </c>
+      <c r="B226" s="5" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="227" spans="1:2" ht="15.5">
+      <c r="A227" t="s">
+        <v>15</v>
+      </c>
+      <c r="B227" s="5" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="228" spans="1:2" ht="15.5">
+      <c r="A228" t="s">
+        <v>15</v>
+      </c>
+      <c r="B228" s="5" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="229" spans="1:2" ht="15.5">
+      <c r="A229" t="s">
+        <v>15</v>
+      </c>
+      <c r="B229" s="5" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="230" spans="1:2" ht="15.5">
+      <c r="A230" t="s">
+        <v>15</v>
+      </c>
+      <c r="B230" s="5" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="231" spans="1:2" ht="15.5">
+      <c r="A231" t="s">
+        <v>15</v>
+      </c>
+      <c r="B231" s="5" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="232" spans="1:2" ht="15.5">
+      <c r="A232" t="s">
+        <v>15</v>
+      </c>
+      <c r="B232" s="5" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="233" spans="1:2" ht="15.5">
+      <c r="A233" t="s">
+        <v>15</v>
+      </c>
+      <c r="B233" s="5" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="234" spans="1:2" ht="15.5">
+      <c r="A234" t="s">
+        <v>15</v>
+      </c>
+      <c r="B234" s="5" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="235" spans="1:2" ht="15.5">
+      <c r="A235" t="s">
+        <v>15</v>
+      </c>
+      <c r="B235" s="5" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="236" spans="1:2" ht="15.5">
+      <c r="A236" t="s">
+        <v>15</v>
+      </c>
+      <c r="B236" s="5" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="237" spans="1:2" ht="15.5">
+      <c r="A237" t="s">
+        <v>15</v>
+      </c>
+      <c r="B237" s="5" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="238" spans="1:2" ht="15.5">
+      <c r="A238" t="s">
+        <v>15</v>
+      </c>
+      <c r="B238" s="5" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="239" spans="1:2" ht="15.5">
+      <c r="A239" t="s">
+        <v>15</v>
+      </c>
+      <c r="B239" s="5" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="240" spans="1:2" ht="15.5">
+      <c r="A240" t="s">
+        <v>15</v>
+      </c>
+      <c r="B240" s="5" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="241" spans="1:2" ht="15.5">
+      <c r="A241" t="s">
+        <v>15</v>
+      </c>
+      <c r="B241" s="5" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="242" spans="1:2" ht="15.5">
+      <c r="A242" t="s">
+        <v>15</v>
+      </c>
+      <c r="B242" s="5" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="243" spans="1:2" ht="15.5">
+      <c r="A243" t="s">
+        <v>15</v>
+      </c>
+      <c r="B243" s="5" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="244" spans="1:2" ht="15.5">
+      <c r="A244" t="s">
+        <v>15</v>
+      </c>
+      <c r="B244" s="5" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="245" spans="1:2" ht="15.5">
+      <c r="A245" t="s">
+        <v>15</v>
+      </c>
+      <c r="B245" s="5" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="246" spans="1:2" ht="15.5">
+      <c r="A246" t="s">
+        <v>15</v>
+      </c>
+      <c r="B246" s="5" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="247" spans="1:2" ht="15.5">
+      <c r="A247" t="s">
+        <v>15</v>
+      </c>
+      <c r="B247" s="5" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="248" spans="1:2" ht="15.5">
+      <c r="A248" t="s">
+        <v>15</v>
+      </c>
+      <c r="B248" s="5" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="249" spans="1:2" ht="15.5">
+      <c r="A249" t="s">
+        <v>15</v>
+      </c>
+      <c r="B249" s="5" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="250" spans="1:2" ht="15.5">
+      <c r="A250" t="s">
+        <v>15</v>
+      </c>
+      <c r="B250" s="5" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="251" spans="1:2" ht="15.5">
+      <c r="A251" t="s">
+        <v>15</v>
+      </c>
+      <c r="B251" s="5" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="252" spans="1:2" ht="15.5">
+      <c r="A252" t="s">
+        <v>15</v>
+      </c>
+      <c r="B252" s="5" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="253" spans="1:2" ht="15.5">
+      <c r="A253" t="s">
+        <v>15</v>
+      </c>
+      <c r="B253" s="5" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="254" spans="1:2" ht="15.5">
+      <c r="A254" t="s">
+        <v>15</v>
+      </c>
+      <c r="B254" s="5" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="255" spans="1:2" ht="15.5">
+      <c r="A255" t="s">
+        <v>15</v>
+      </c>
+      <c r="B255" s="5" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="256" spans="1:2" ht="15.5">
+      <c r="A256" t="s">
+        <v>15</v>
+      </c>
+      <c r="B256" s="5" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="257" spans="1:2" ht="15.5">
+      <c r="A257" t="s">
+        <v>15</v>
+      </c>
+      <c r="B257" s="5" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="258" spans="1:2" ht="15.5">
+      <c r="A258" t="s">
+        <v>15</v>
+      </c>
+      <c r="B258" s="5" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="259" spans="1:2" ht="15.5">
+      <c r="A259" t="s">
+        <v>15</v>
+      </c>
+      <c r="B259" s="5" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="260" spans="1:2" ht="15.5">
+      <c r="A260" t="s">
+        <v>15</v>
+      </c>
+      <c r="B260" s="5" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="261" spans="1:2" ht="15.5">
+      <c r="A261" t="s">
+        <v>15</v>
+      </c>
+      <c r="B261" s="5" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="262" spans="1:2" ht="15.5">
+      <c r="A262" t="s">
+        <v>15</v>
+      </c>
+      <c r="B262" s="5" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="263" spans="1:2" ht="15.5">
+      <c r="A263" t="s">
+        <v>15</v>
+      </c>
+      <c r="B263" s="5" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="264" spans="1:2" ht="15.5">
+      <c r="A264" t="s">
+        <v>15</v>
+      </c>
+      <c r="B264" s="5" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="265" spans="1:2" ht="15.5">
+      <c r="A265" t="s">
+        <v>15</v>
+      </c>
+      <c r="B265" s="5" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="266" spans="1:2" ht="15.5">
+      <c r="A266" t="s">
+        <v>15</v>
+      </c>
+      <c r="B266" s="5" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="267" spans="1:2" ht="15.5">
+      <c r="A267" t="s">
+        <v>15</v>
+      </c>
+      <c r="B267" s="5" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="268" spans="1:2" ht="15.5">
+      <c r="A268" t="s">
+        <v>15</v>
+      </c>
+      <c r="B268" s="5" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="269" spans="1:2" ht="15.5">
+      <c r="A269" t="s">
+        <v>15</v>
+      </c>
+      <c r="B269" s="5" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="270" spans="1:2" ht="15.5">
+      <c r="A270" t="s">
+        <v>15</v>
+      </c>
+      <c r="B270" s="5" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="271" spans="1:2" ht="15.5">
+      <c r="A271" t="s">
+        <v>15</v>
+      </c>
+      <c r="B271" s="5" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="272" spans="1:2" ht="15.5">
+      <c r="A272" t="s">
+        <v>15</v>
+      </c>
+      <c r="B272" s="5" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="273" spans="1:2" ht="15.5">
+      <c r="A273" t="s">
+        <v>15</v>
+      </c>
+      <c r="B273" s="5" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="274" spans="1:2" ht="15.5">
+      <c r="A274" t="s">
+        <v>15</v>
+      </c>
+      <c r="B274" s="5" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="275" spans="1:2" ht="15.5">
+      <c r="A275" t="s">
+        <v>15</v>
+      </c>
+      <c r="B275" s="5" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="276" spans="1:2" ht="15.5">
+      <c r="A276" t="s">
+        <v>15</v>
+      </c>
+      <c r="B276" s="5" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="277" spans="1:2" ht="15.5">
+      <c r="A277" t="s">
+        <v>15</v>
+      </c>
+      <c r="B277" s="5" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="278" spans="1:2" ht="15.5">
+      <c r="A278" t="s">
+        <v>15</v>
+      </c>
+      <c r="B278" s="5" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="279" spans="1:2" ht="15.5">
+      <c r="A279" t="s">
+        <v>15</v>
+      </c>
+      <c r="B279" s="5" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="280" spans="1:2" ht="15.5">
+      <c r="A280" t="s">
+        <v>15</v>
+      </c>
+      <c r="B280" s="5" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="281" spans="1:2" ht="15.5">
+      <c r="A281" t="s">
+        <v>15</v>
+      </c>
+      <c r="B281" s="5" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="282" spans="1:2" ht="15.5">
+      <c r="A282" t="s">
+        <v>15</v>
+      </c>
+      <c r="B282" s="5" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="283" spans="1:2" ht="15.5">
+      <c r="A283" t="s">
+        <v>15</v>
+      </c>
+      <c r="B283" s="5" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="284" spans="1:2" ht="15.5">
+      <c r="A284" t="s">
+        <v>15</v>
+      </c>
+      <c r="B284" s="5" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="285" spans="1:2" ht="15.5">
+      <c r="A285" t="s">
+        <v>15</v>
+      </c>
+      <c r="B285" s="5" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="286" spans="1:2" ht="15.5">
+      <c r="A286" t="s">
+        <v>15</v>
+      </c>
+      <c r="B286" s="5" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="287" spans="1:2" ht="15.5">
+      <c r="A287" t="s">
+        <v>15</v>
+      </c>
+      <c r="B287" s="5" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="288" spans="1:2" ht="15.5">
+      <c r="A288" t="s">
+        <v>15</v>
+      </c>
+      <c r="B288" s="5" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="289" spans="1:2" ht="15.5">
+      <c r="A289" t="s">
+        <v>15</v>
+      </c>
+      <c r="B289" s="5" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="290" spans="1:2" ht="15.5">
+      <c r="A290" t="s">
+        <v>15</v>
+      </c>
+      <c r="B290" s="5" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="291" spans="1:2" ht="15.5">
+      <c r="A291" t="s">
+        <v>15</v>
+      </c>
+      <c r="B291" s="5" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="292" spans="1:2" ht="15.5">
+      <c r="A292" t="s">
+        <v>15</v>
+      </c>
+      <c r="B292" s="5" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="293" spans="1:2" ht="15.5">
+      <c r="A293" t="s">
+        <v>15</v>
+      </c>
+      <c r="B293" s="5" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="294" spans="1:2" ht="15.5">
+      <c r="A294" t="s">
+        <v>15</v>
+      </c>
+      <c r="B294" s="5" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="295" spans="1:2" ht="15.5">
+      <c r="A295" t="s">
+        <v>15</v>
+      </c>
+      <c r="B295" s="5" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="296" spans="1:2" ht="15.5">
+      <c r="A296" t="s">
+        <v>15</v>
+      </c>
+      <c r="B296" s="5" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="297" spans="1:2" ht="15.5">
+      <c r="A297" t="s">
+        <v>15</v>
+      </c>
+      <c r="B297" s="5" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="298" spans="1:2" ht="15.5">
+      <c r="A298" t="s">
+        <v>15</v>
+      </c>
+      <c r="B298" s="5" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="299" spans="1:2" ht="15.5">
+      <c r="A299" t="s">
+        <v>15</v>
+      </c>
+      <c r="B299" s="5" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="300" spans="1:2" ht="15.5">
+      <c r="A300" t="s">
+        <v>15</v>
+      </c>
+      <c r="B300" s="5" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="301" spans="1:2" ht="15.5">
+      <c r="A301" t="s">
+        <v>15</v>
+      </c>
+      <c r="B301" s="5" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="302" spans="1:2" ht="15.5">
+      <c r="A302" t="s">
+        <v>15</v>
+      </c>
+      <c r="B302" s="5" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="303" spans="1:2" ht="15.5">
+      <c r="A303" t="s">
+        <v>15</v>
+      </c>
+      <c r="B303" s="5" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="304" spans="1:2" ht="15.5">
+      <c r="A304" t="s">
+        <v>15</v>
+      </c>
+      <c r="B304" s="5" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="305" spans="1:2" ht="15.5">
+      <c r="A305" t="s">
+        <v>15</v>
+      </c>
+      <c r="B305" s="5" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="306" spans="1:2" ht="15.5">
+      <c r="A306" t="s">
+        <v>15</v>
+      </c>
+      <c r="B306" s="5" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="307" spans="1:2" ht="15.5">
+      <c r="A307" t="s">
+        <v>15</v>
+      </c>
+      <c r="B307" s="5" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="308" spans="1:2" ht="15.5">
+      <c r="A308" t="s">
+        <v>15</v>
+      </c>
+      <c r="B308" s="5" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="309" spans="1:2" ht="15.5">
+      <c r="A309" t="s">
+        <v>15</v>
+      </c>
+      <c r="B309" s="5" t="s">
+        <v>175</v>
       </c>
     </row>
   </sheetData>
@@ -1778,6 +3780,23 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="32f52b41-3b94-4090-a175-52d6bdf443eb" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100D4CAC9FC675B57408E93BF556641D4D2" ma:contentTypeVersion="12" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="274a8390434e2b99e5c0abfa3a3bc86a">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="32f52b41-3b94-4090-a175-52d6bdf443eb" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="396c0ffd131d9db66c00cc10498a82b8" ns3:_="">
     <xsd:import namespace="32f52b41-3b94-4090-a175-52d6bdf443eb"/>
@@ -1971,24 +3990,31 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E0E37CA3-E383-451B-A722-9F0EA8A56E91}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="32f52b41-3b94-4090-a175-52d6bdf443eb"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="32f52b41-3b94-4090-a175-52d6bdf443eb" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5CE60954-2BCD-4F54-AE55-7D46BDC4758B}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{77BA3598-10A6-4EE4-9EA0-3517074D3A96}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2004,28 +4030,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5CE60954-2BCD-4F54-AE55-7D46BDC4758B}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E0E37CA3-E383-451B-A722-9F0EA8A56E91}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="32f52b41-3b94-4090-a175-52d6bdf443eb"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
📊 Update Excel files from OneDrive - 2025-09-12 09:41:11
</commit_message>
<xml_diff>
--- a/backend/data/Spare_Parts_Inventory.xlsx
+++ b/backend/data/Spare_Parts_Inventory.xlsx
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="135" documentId="8_{DFEF1166-70E6-421A-ABBC-F474D4E5088C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1C4F2F95-3B2A-4137-BE3D-951D4A2B4B29}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{72449171-FCEF-49D6-AEAC-5AACDA2C6B26}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{72449171-FCEF-49D6-AEAC-5AACDA2C6B26}"/>
   </bookViews>
   <sheets>
     <sheet name="Spare_Parts_Inventory" sheetId="1" r:id="rId1"/>
@@ -920,7 +920,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1261,8 +1261,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{94C1C842-7533-49D8-BD7E-9BF474738299}">
   <dimension ref="A1:L310"/>
   <sheetViews>
-    <sheetView zoomScale="79" workbookViewId="0">
-      <selection activeCell="A72" sqref="A72:B310"/>
+    <sheetView tabSelected="1" zoomScale="79" workbookViewId="0">
+      <selection activeCell="K11" sqref="K11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -3807,7 +3807,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{140D0306-11E7-4EAC-BF2E-8F375561574C}">
   <dimension ref="A1:C241"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
@@ -6480,15 +6480,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100D4CAC9FC675B57408E93BF556641D4D2" ma:contentTypeVersion="12" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="274a8390434e2b99e5c0abfa3a3bc86a">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="32f52b41-3b94-4090-a175-52d6bdf443eb" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="396c0ffd131d9db66c00cc10498a82b8" ns3:_="">
     <xsd:import namespace="32f52b41-3b94-4090-a175-52d6bdf443eb"/>
@@ -6682,31 +6673,32 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E0E37CA3-E383-451B-A722-9F0EA8A56E91}">
   <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="32f52b41-3b94-4090-a175-52d6bdf443eb"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="32f52b41-3b94-4090-a175-52d6bdf443eb"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5CE60954-2BCD-4F54-AE55-7D46BDC4758B}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{77BA3598-10A6-4EE4-9EA0-3517074D3A96}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -6722,4 +6714,12 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5CE60954-2BCD-4F54-AE55-7D46BDC4758B}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
📊 Update Excel files from OneDrive - 2025-09-16 09:43:11
</commit_message>
<xml_diff>
--- a/backend/data/Spare_Parts_Inventory.xlsx
+++ b/backend/data/Spare_Parts_Inventory.xlsx
@@ -8,13 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://vikramsolar0-my.sharepoint.com/personal/naveen_chamaria_vikramsolar_com/Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="135" documentId="8_{DFEF1166-70E6-421A-ABBC-F474D4E5088C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1C4F2F95-3B2A-4137-BE3D-951D4A2B4B29}"/>
+  <xr:revisionPtr revIDLastSave="65" documentId="8_{319E19CD-5EDD-431C-9D80-979664711085}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7BB2E0D2-A44E-4B79-B29F-7F623E85B3FA}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{72449171-FCEF-49D6-AEAC-5AACDA2C6B26}"/>
   </bookViews>
   <sheets>
     <sheet name="Spare_Parts_Inventory" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -37,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1111" uniqueCount="271">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="628" uniqueCount="267">
   <si>
     <t>Equipment_Category</t>
   </si>
@@ -141,9 +140,6 @@
     <t>Tension transmitter</t>
   </si>
   <si>
-    <t>Thermocouples</t>
-  </si>
-  <si>
     <t>24V switching power supply</t>
   </si>
   <si>
@@ -841,15 +837,6 @@
   </si>
   <si>
     <t>Battery AA</t>
-  </si>
-  <si>
-    <t>EQUIPMENT NAME</t>
-  </si>
-  <si>
-    <t>ASSOCIATED SPARE PARTS NAME</t>
-  </si>
-  <si>
-    <t>SERIAL NO. OF EQUIPMENT</t>
   </si>
 </sst>
 </file>
@@ -1259,10 +1246,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{94C1C842-7533-49D8-BD7E-9BF474738299}">
-  <dimension ref="A1:L310"/>
+  <dimension ref="A1:L309"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="79" workbookViewId="0">
-      <selection activeCell="K11" sqref="K11"/>
+    <sheetView tabSelected="1" topLeftCell="A57" zoomScale="82" workbookViewId="0">
+      <selection activeCell="F66" sqref="F66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -1325,6 +1312,9 @@
       <c r="B2" s="3" t="s">
         <v>18</v>
       </c>
+      <c r="F2">
+        <v>0</v>
+      </c>
     </row>
     <row r="3" spans="1:12">
       <c r="A3" t="s">
@@ -1333,6 +1323,9 @@
       <c r="B3" s="3" t="s">
         <v>19</v>
       </c>
+      <c r="F3">
+        <v>0</v>
+      </c>
     </row>
     <row r="4" spans="1:12">
       <c r="A4" t="s">
@@ -1341,6 +1334,9 @@
       <c r="B4" s="3" t="s">
         <v>20</v>
       </c>
+      <c r="F4">
+        <v>1</v>
+      </c>
     </row>
     <row r="5" spans="1:12">
       <c r="A5" t="s">
@@ -1349,6 +1345,9 @@
       <c r="B5" s="3" t="s">
         <v>21</v>
       </c>
+      <c r="F5">
+        <v>1</v>
+      </c>
     </row>
     <row r="6" spans="1:12">
       <c r="A6" t="s">
@@ -1357,6 +1356,9 @@
       <c r="B6" s="3" t="s">
         <v>22</v>
       </c>
+      <c r="F6">
+        <v>1</v>
+      </c>
     </row>
     <row r="7" spans="1:12">
       <c r="A7" t="s">
@@ -1365,6 +1367,9 @@
       <c r="B7" s="3" t="s">
         <v>23</v>
       </c>
+      <c r="F7">
+        <v>1</v>
+      </c>
     </row>
     <row r="8" spans="1:12">
       <c r="A8" t="s">
@@ -1373,6 +1378,9 @@
       <c r="B8" s="3" t="s">
         <v>24</v>
       </c>
+      <c r="F8">
+        <v>0</v>
+      </c>
     </row>
     <row r="9" spans="1:12">
       <c r="A9" t="s">
@@ -1381,6 +1389,9 @@
       <c r="B9" s="3" t="s">
         <v>25</v>
       </c>
+      <c r="F9">
+        <v>0</v>
+      </c>
     </row>
     <row r="10" spans="1:12">
       <c r="A10" t="s">
@@ -1389,6 +1400,9 @@
       <c r="B10" s="3" t="s">
         <v>26</v>
       </c>
+      <c r="F10">
+        <v>0</v>
+      </c>
     </row>
     <row r="11" spans="1:12">
       <c r="A11" t="s">
@@ -1397,6 +1411,9 @@
       <c r="B11" s="3" t="s">
         <v>27</v>
       </c>
+      <c r="F11">
+        <v>0</v>
+      </c>
     </row>
     <row r="12" spans="1:12">
       <c r="A12" t="s">
@@ -1405,6 +1422,9 @@
       <c r="B12" s="3" t="s">
         <v>28</v>
       </c>
+      <c r="F12">
+        <v>0</v>
+      </c>
     </row>
     <row r="13" spans="1:12">
       <c r="A13" t="s">
@@ -1413,6 +1433,9 @@
       <c r="B13" s="3" t="s">
         <v>29</v>
       </c>
+      <c r="F13">
+        <v>0</v>
+      </c>
     </row>
     <row r="14" spans="1:12">
       <c r="A14" t="s">
@@ -1421,6 +1444,9 @@
       <c r="B14" s="3" t="s">
         <v>30</v>
       </c>
+      <c r="F14">
+        <v>1</v>
+      </c>
     </row>
     <row r="15" spans="1:12">
       <c r="A15" t="s">
@@ -1429,6 +1455,9 @@
       <c r="B15" s="3" t="s">
         <v>31</v>
       </c>
+      <c r="F15">
+        <v>0</v>
+      </c>
     </row>
     <row r="16" spans="1:12">
       <c r="A16" t="s">
@@ -1437,128 +1466,176 @@
       <c r="B16" s="3" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="17" spans="1:2">
+      <c r="F16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6">
       <c r="A17" t="s">
         <v>13</v>
       </c>
       <c r="B17" s="3" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="18" spans="1:2">
+      <c r="F17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6">
       <c r="A18" t="s">
         <v>13</v>
       </c>
       <c r="B18" s="3" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="19" spans="1:2">
+      <c r="F18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6">
       <c r="A19" t="s">
         <v>13</v>
       </c>
       <c r="B19" s="3" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="20" spans="1:2">
+      <c r="F19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6">
       <c r="A20" t="s">
         <v>13</v>
       </c>
       <c r="B20" s="3" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="21" spans="1:2">
+      <c r="F20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6">
       <c r="A21" t="s">
         <v>13</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2">
+        <v>80</v>
+      </c>
+      <c r="F21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6">
       <c r="A22" t="s">
         <v>13</v>
       </c>
       <c r="B22" s="3" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="23" spans="1:2">
+      <c r="F22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6">
       <c r="A23" t="s">
         <v>13</v>
       </c>
       <c r="B23" s="3" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="24" spans="1:2">
+      <c r="F23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6">
       <c r="A24" t="s">
         <v>13</v>
       </c>
       <c r="B24" s="3" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="25" spans="1:2">
+      <c r="F24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6">
       <c r="A25" t="s">
         <v>13</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2">
+        <v>37</v>
+      </c>
+      <c r="F25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6">
       <c r="A26" t="s">
         <v>13</v>
       </c>
       <c r="B26" s="3" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="27" spans="1:2">
+      <c r="F26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6">
       <c r="A27" t="s">
         <v>13</v>
       </c>
       <c r="B27" s="3" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="28" spans="1:2">
+      <c r="F27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6">
       <c r="A28" t="s">
         <v>13</v>
       </c>
       <c r="B28" s="3" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="29" spans="1:2">
+      <c r="F28">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6">
       <c r="A29" t="s">
         <v>13</v>
       </c>
       <c r="B29" s="3" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="30" spans="1:2">
+      <c r="F29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6">
       <c r="A30" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B30" s="3" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="31" spans="1:2">
+      <c r="F30">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6">
       <c r="A31" t="s">
         <v>12</v>
       </c>
       <c r="B31" s="3" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="32" spans="1:2">
+      <c r="F31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6">
       <c r="A32" t="s">
         <v>12</v>
       </c>
@@ -1566,31 +1643,40 @@
         <v>44</v>
       </c>
     </row>
-    <row r="33" spans="1:2">
+    <row r="33" spans="1:6">
       <c r="A33" t="s">
         <v>12</v>
       </c>
       <c r="B33" s="3" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="34" spans="1:2">
+      <c r="F33">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6">
       <c r="A34" t="s">
         <v>12</v>
       </c>
       <c r="B34" s="3" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="35" spans="1:2">
+      <c r="F34">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6">
       <c r="A35" t="s">
         <v>12</v>
       </c>
       <c r="B35" s="3" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="36" spans="1:2">
+      <c r="F35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6">
       <c r="A36" t="s">
         <v>12</v>
       </c>
@@ -1598,247 +1684,334 @@
         <v>48</v>
       </c>
     </row>
-    <row r="37" spans="1:2">
+    <row r="37" spans="1:6">
       <c r="A37" t="s">
         <v>12</v>
       </c>
       <c r="B37" s="3" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="38" spans="1:2">
+      <c r="F37">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6">
       <c r="A38" t="s">
         <v>12</v>
       </c>
       <c r="B38" s="3" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="39" spans="1:2">
+      <c r="F38">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6">
       <c r="A39" t="s">
         <v>12</v>
       </c>
       <c r="B39" s="3" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="40" spans="1:2">
+      <c r="F39">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6">
       <c r="A40" t="s">
         <v>12</v>
       </c>
       <c r="B40" s="3" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="41" spans="1:2">
+      <c r="F40">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6">
       <c r="A41" t="s">
         <v>12</v>
       </c>
       <c r="B41" s="3" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="42" spans="1:2">
+      <c r="F41">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6">
       <c r="A42" t="s">
         <v>12</v>
       </c>
       <c r="B42" s="3" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="43" spans="1:2">
+      <c r="F42">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6">
       <c r="A43" t="s">
         <v>12</v>
       </c>
       <c r="B43" s="3" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="44" spans="1:2">
+      <c r="F43">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6">
       <c r="A44" t="s">
         <v>12</v>
       </c>
       <c r="B44" s="3" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="45" spans="1:2">
+      <c r="F44">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6">
       <c r="A45" t="s">
         <v>12</v>
       </c>
       <c r="B45" s="3" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="46" spans="1:2">
+      <c r="F45">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6">
       <c r="A46" t="s">
         <v>12</v>
       </c>
       <c r="B46" s="3" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="47" spans="1:2">
+      <c r="F46">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6">
       <c r="A47" t="s">
         <v>12</v>
       </c>
       <c r="B47" s="3" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="48" spans="1:2">
+      <c r="F47">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6">
       <c r="A48" t="s">
         <v>12</v>
       </c>
       <c r="B48" s="3" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="49" spans="1:2">
+      <c r="F48">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6">
       <c r="A49" t="s">
         <v>12</v>
       </c>
       <c r="B49" s="3" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="50" spans="1:2">
+        <v>25</v>
+      </c>
+      <c r="F49">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6">
       <c r="A50" t="s">
         <v>12</v>
       </c>
       <c r="B50" s="3" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="51" spans="1:2">
+        <v>61</v>
+      </c>
+      <c r="F50">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6">
       <c r="A51" t="s">
         <v>12</v>
       </c>
       <c r="B51" s="3" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="52" spans="1:2">
+      <c r="F51">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6">
       <c r="A52" t="s">
         <v>12</v>
       </c>
       <c r="B52" s="3" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="53" spans="1:2">
+      <c r="F52">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6">
       <c r="A53" t="s">
         <v>12</v>
       </c>
       <c r="B53" s="3" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="54" spans="1:2">
+      <c r="F53">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6">
       <c r="A54" t="s">
         <v>12</v>
       </c>
       <c r="B54" s="3" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="55" spans="1:2">
+      <c r="F54">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6">
       <c r="A55" t="s">
         <v>12</v>
       </c>
       <c r="B55" s="3" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="56" spans="1:2">
+      <c r="F55">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6">
       <c r="A56" t="s">
         <v>12</v>
       </c>
       <c r="B56" s="3" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="57" spans="1:2">
+      <c r="F56">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6">
       <c r="A57" t="s">
         <v>12</v>
       </c>
       <c r="B57" s="3" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="58" spans="1:2">
+      <c r="F57">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6">
       <c r="A58" t="s">
         <v>12</v>
       </c>
       <c r="B58" s="3" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="59" spans="1:2">
+      <c r="F58">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6">
       <c r="A59" t="s">
         <v>12</v>
       </c>
       <c r="B59" s="3" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="60" spans="1:2">
+      <c r="F59">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6">
       <c r="A60" t="s">
         <v>12</v>
       </c>
       <c r="B60" s="3" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="61" spans="1:2">
+      <c r="F60">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6">
       <c r="A61" t="s">
         <v>12</v>
       </c>
       <c r="B61" s="3" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="62" spans="1:2">
+      <c r="F61">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6">
       <c r="A62" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="B62" s="3" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="63" spans="1:2">
+      <c r="F62">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" ht="17">
       <c r="A63" t="s">
-        <v>16</v>
-      </c>
-      <c r="B63" s="3" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="64" spans="1:2" ht="17">
+        <v>17</v>
+      </c>
+      <c r="B63" s="4" t="s">
+        <v>266</v>
+      </c>
+      <c r="F63">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" ht="17">
       <c r="A64" t="s">
         <v>17</v>
       </c>
       <c r="B64" s="4" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="65" spans="1:2" ht="17">
+        <v>265</v>
+      </c>
+      <c r="F64">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" ht="17">
       <c r="A65" t="s">
         <v>17</v>
       </c>
       <c r="B65" s="4" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="66" spans="1:2" ht="17">
+        <v>79</v>
+      </c>
+      <c r="F65">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" ht="17">
       <c r="A66" t="s">
         <v>17</v>
       </c>
       <c r="B66" s="4" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="67" spans="1:2" ht="17">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" ht="17">
       <c r="A67" t="s">
         <v>17</v>
       </c>
@@ -1846,7 +2019,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="68" spans="1:2" ht="17">
+    <row r="68" spans="1:6" ht="17">
       <c r="A68" t="s">
         <v>17</v>
       </c>
@@ -1854,7 +2027,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="69" spans="1:2" ht="17">
+    <row r="69" spans="1:6" ht="17">
       <c r="A69" t="s">
         <v>17</v>
       </c>
@@ -1862,7 +2035,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="70" spans="1:2" ht="17">
+    <row r="70" spans="1:6" ht="17">
       <c r="A70" t="s">
         <v>17</v>
       </c>
@@ -1870,15 +2043,15 @@
         <v>78</v>
       </c>
     </row>
-    <row r="71" spans="1:2" ht="17">
+    <row r="71" spans="1:6" ht="15.5">
       <c r="A71" t="s">
-        <v>17</v>
-      </c>
-      <c r="B71" s="4" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="72" spans="1:2" ht="15.5">
+        <v>14</v>
+      </c>
+      <c r="B71" s="5" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6" ht="15.5">
       <c r="A72" t="s">
         <v>14</v>
       </c>
@@ -1886,7 +2059,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="73" spans="1:2" ht="15.5">
+    <row r="73" spans="1:6" ht="15.5">
       <c r="A73" t="s">
         <v>14</v>
       </c>
@@ -1894,15 +2067,15 @@
         <v>86</v>
       </c>
     </row>
-    <row r="74" spans="1:2" ht="15.5">
+    <row r="74" spans="1:6" ht="15.5">
       <c r="A74" t="s">
         <v>14</v>
       </c>
       <c r="B74" s="5" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="75" spans="1:2" ht="15.5">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6" ht="15.5">
       <c r="A75" t="s">
         <v>14</v>
       </c>
@@ -1910,23 +2083,23 @@
         <v>175</v>
       </c>
     </row>
-    <row r="76" spans="1:2" ht="15.5">
+    <row r="76" spans="1:6" ht="15.5">
       <c r="A76" t="s">
         <v>14</v>
       </c>
       <c r="B76" s="5" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6" ht="15.5">
+      <c r="A77" t="s">
+        <v>14</v>
+      </c>
+      <c r="B77" s="5" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="77" spans="1:2" ht="15.5">
-      <c r="A77" t="s">
-        <v>14</v>
-      </c>
-      <c r="B77" s="5" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="78" spans="1:2" ht="15.5">
+    <row r="78" spans="1:6" ht="15.5">
       <c r="A78" t="s">
         <v>14</v>
       </c>
@@ -1934,15 +2107,15 @@
         <v>177</v>
       </c>
     </row>
-    <row r="79" spans="1:2" ht="15.5">
+    <row r="79" spans="1:6" ht="15.5">
       <c r="A79" t="s">
         <v>14</v>
       </c>
       <c r="B79" s="5" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="80" spans="1:2" ht="15.5">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6" ht="15.5">
       <c r="A80" t="s">
         <v>14</v>
       </c>
@@ -1963,7 +2136,7 @@
         <v>14</v>
       </c>
       <c r="B82" s="5" t="s">
-        <v>91</v>
+        <v>178</v>
       </c>
     </row>
     <row r="83" spans="1:2" ht="15.5">
@@ -2043,7 +2216,7 @@
         <v>14</v>
       </c>
       <c r="B92" s="5" t="s">
-        <v>188</v>
+        <v>100</v>
       </c>
     </row>
     <row r="93" spans="1:2" ht="15.5">
@@ -2059,7 +2232,7 @@
         <v>14</v>
       </c>
       <c r="B94" s="5" t="s">
-        <v>102</v>
+        <v>188</v>
       </c>
     </row>
     <row r="95" spans="1:2" ht="15.5">
@@ -2083,7 +2256,7 @@
         <v>14</v>
       </c>
       <c r="B97" s="5" t="s">
-        <v>191</v>
+        <v>97</v>
       </c>
     </row>
     <row r="98" spans="1:2" ht="15.5">
@@ -2099,7 +2272,7 @@
         <v>14</v>
       </c>
       <c r="B99" s="5" t="s">
-        <v>99</v>
+        <v>191</v>
       </c>
     </row>
     <row r="100" spans="1:2" ht="15.5">
@@ -2107,7 +2280,7 @@
         <v>14</v>
       </c>
       <c r="B100" s="5" t="s">
-        <v>192</v>
+        <v>102</v>
       </c>
     </row>
     <row r="101" spans="1:2" ht="15.5">
@@ -2115,7 +2288,7 @@
         <v>14</v>
       </c>
       <c r="B101" s="5" t="s">
-        <v>103</v>
+        <v>192</v>
       </c>
     </row>
     <row r="102" spans="1:2" ht="15.5">
@@ -2171,7 +2344,7 @@
         <v>14</v>
       </c>
       <c r="B108" s="5" t="s">
-        <v>199</v>
+        <v>138</v>
       </c>
     </row>
     <row r="109" spans="1:2" ht="15.5">
@@ -2179,7 +2352,7 @@
         <v>14</v>
       </c>
       <c r="B109" s="5" t="s">
-        <v>139</v>
+        <v>103</v>
       </c>
     </row>
     <row r="110" spans="1:2" ht="15.5">
@@ -2203,7 +2376,7 @@
         <v>14</v>
       </c>
       <c r="B112" s="5" t="s">
-        <v>106</v>
+        <v>199</v>
       </c>
     </row>
     <row r="113" spans="1:2" ht="15.5">
@@ -2219,7 +2392,7 @@
         <v>14</v>
       </c>
       <c r="B114" s="5" t="s">
-        <v>201</v>
+        <v>109</v>
       </c>
     </row>
     <row r="115" spans="1:2" ht="15.5">
@@ -2227,7 +2400,7 @@
         <v>14</v>
       </c>
       <c r="B115" s="5" t="s">
-        <v>110</v>
+        <v>201</v>
       </c>
     </row>
     <row r="116" spans="1:2" ht="15.5">
@@ -2275,7 +2448,7 @@
         <v>14</v>
       </c>
       <c r="B121" s="5" t="s">
-        <v>207</v>
+        <v>118</v>
       </c>
     </row>
     <row r="122" spans="1:2" ht="15.5">
@@ -2283,7 +2456,7 @@
         <v>14</v>
       </c>
       <c r="B122" s="5" t="s">
-        <v>119</v>
+        <v>110</v>
       </c>
     </row>
     <row r="123" spans="1:2" ht="15.5">
@@ -2291,7 +2464,7 @@
         <v>14</v>
       </c>
       <c r="B123" s="5" t="s">
-        <v>111</v>
+        <v>127</v>
       </c>
     </row>
     <row r="124" spans="1:2" ht="15.5">
@@ -2307,7 +2480,7 @@
         <v>14</v>
       </c>
       <c r="B125" s="5" t="s">
-        <v>129</v>
+        <v>111</v>
       </c>
     </row>
     <row r="126" spans="1:2" ht="15.5">
@@ -2315,7 +2488,7 @@
         <v>14</v>
       </c>
       <c r="B126" s="5" t="s">
-        <v>112</v>
+        <v>207</v>
       </c>
     </row>
     <row r="127" spans="1:2" ht="15.5">
@@ -2323,7 +2496,7 @@
         <v>14</v>
       </c>
       <c r="B127" s="5" t="s">
-        <v>208</v>
+        <v>149</v>
       </c>
     </row>
     <row r="128" spans="1:2" ht="15.5">
@@ -2339,7 +2512,7 @@
         <v>14</v>
       </c>
       <c r="B129" s="5" t="s">
-        <v>151</v>
+        <v>112</v>
       </c>
     </row>
     <row r="130" spans="1:2" ht="15.5">
@@ -2347,7 +2520,7 @@
         <v>14</v>
       </c>
       <c r="B130" s="5" t="s">
-        <v>113</v>
+        <v>208</v>
       </c>
     </row>
     <row r="131" spans="1:2" ht="15.5">
@@ -2363,7 +2536,7 @@
         <v>14</v>
       </c>
       <c r="B132" s="5" t="s">
-        <v>210</v>
+        <v>113</v>
       </c>
     </row>
     <row r="133" spans="1:2" ht="15.5">
@@ -2371,7 +2544,7 @@
         <v>14</v>
       </c>
       <c r="B133" s="5" t="s">
-        <v>114</v>
+        <v>134</v>
       </c>
     </row>
     <row r="134" spans="1:2" ht="15.5">
@@ -2379,7 +2552,7 @@
         <v>14</v>
       </c>
       <c r="B134" s="5" t="s">
-        <v>135</v>
+        <v>210</v>
       </c>
     </row>
     <row r="135" spans="1:2" ht="15.5">
@@ -2387,7 +2560,7 @@
         <v>14</v>
       </c>
       <c r="B135" s="5" t="s">
-        <v>211</v>
+        <v>114</v>
       </c>
     </row>
     <row r="136" spans="1:2" ht="15.5">
@@ -2395,7 +2568,7 @@
         <v>14</v>
       </c>
       <c r="B136" s="5" t="s">
-        <v>115</v>
+        <v>211</v>
       </c>
     </row>
     <row r="137" spans="1:2" ht="15.5">
@@ -2403,7 +2576,7 @@
         <v>14</v>
       </c>
       <c r="B137" s="5" t="s">
-        <v>212</v>
+        <v>131</v>
       </c>
     </row>
     <row r="138" spans="1:2" ht="15.5">
@@ -2411,7 +2584,7 @@
         <v>14</v>
       </c>
       <c r="B138" s="5" t="s">
-        <v>132</v>
+        <v>117</v>
       </c>
     </row>
     <row r="139" spans="1:2" ht="15.5">
@@ -2419,7 +2592,7 @@
         <v>14</v>
       </c>
       <c r="B139" s="5" t="s">
-        <v>118</v>
+        <v>212</v>
       </c>
     </row>
     <row r="140" spans="1:2" ht="15.5">
@@ -2427,7 +2600,7 @@
         <v>14</v>
       </c>
       <c r="B140" s="5" t="s">
-        <v>213</v>
+        <v>115</v>
       </c>
     </row>
     <row r="141" spans="1:2" ht="15.5">
@@ -2443,7 +2616,7 @@
         <v>14</v>
       </c>
       <c r="B142" s="5" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
     </row>
     <row r="143" spans="1:2" ht="15.5">
@@ -2459,7 +2632,7 @@
         <v>14</v>
       </c>
       <c r="B144" s="5" t="s">
-        <v>121</v>
+        <v>213</v>
       </c>
     </row>
     <row r="145" spans="1:2" ht="15.5">
@@ -2467,7 +2640,7 @@
         <v>14</v>
       </c>
       <c r="B145" s="5" t="s">
-        <v>214</v>
+        <v>121</v>
       </c>
     </row>
     <row r="146" spans="1:2" ht="15.5">
@@ -2483,7 +2656,7 @@
         <v>14</v>
       </c>
       <c r="B147" s="5" t="s">
-        <v>123</v>
+        <v>214</v>
       </c>
     </row>
     <row r="148" spans="1:2" ht="15.5">
@@ -2491,7 +2664,7 @@
         <v>14</v>
       </c>
       <c r="B148" s="5" t="s">
-        <v>215</v>
+        <v>123</v>
       </c>
     </row>
     <row r="149" spans="1:2" ht="15.5">
@@ -2499,7 +2672,7 @@
         <v>14</v>
       </c>
       <c r="B149" s="5" t="s">
-        <v>124</v>
+        <v>132</v>
       </c>
     </row>
     <row r="150" spans="1:2" ht="15.5">
@@ -2507,7 +2680,7 @@
         <v>14</v>
       </c>
       <c r="B150" s="5" t="s">
-        <v>133</v>
+        <v>124</v>
       </c>
     </row>
     <row r="151" spans="1:2" ht="15.5">
@@ -2515,7 +2688,7 @@
         <v>14</v>
       </c>
       <c r="B151" s="5" t="s">
-        <v>125</v>
+        <v>215</v>
       </c>
     </row>
     <row r="152" spans="1:2" ht="15.5">
@@ -2523,7 +2696,7 @@
         <v>14</v>
       </c>
       <c r="B152" s="5" t="s">
-        <v>216</v>
+        <v>136</v>
       </c>
     </row>
     <row r="153" spans="1:2" ht="15.5">
@@ -2539,7 +2712,7 @@
         <v>14</v>
       </c>
       <c r="B154" s="5" t="s">
-        <v>138</v>
+        <v>216</v>
       </c>
     </row>
     <row r="155" spans="1:2" ht="15.5">
@@ -2571,7 +2744,7 @@
         <v>14</v>
       </c>
       <c r="B158" s="5" t="s">
-        <v>220</v>
+        <v>139</v>
       </c>
     </row>
     <row r="159" spans="1:2" ht="15.5">
@@ -2579,7 +2752,7 @@
         <v>14</v>
       </c>
       <c r="B159" s="5" t="s">
-        <v>140</v>
+        <v>220</v>
       </c>
     </row>
     <row r="160" spans="1:2" ht="15.5">
@@ -2603,7 +2776,7 @@
         <v>14</v>
       </c>
       <c r="B162" s="5" t="s">
-        <v>223</v>
+        <v>141</v>
       </c>
     </row>
     <row r="163" spans="1:2" ht="15.5">
@@ -2611,7 +2784,7 @@
         <v>14</v>
       </c>
       <c r="B163" s="5" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
     </row>
     <row r="164" spans="1:2" ht="15.5">
@@ -2619,7 +2792,7 @@
         <v>14</v>
       </c>
       <c r="B164" s="5" t="s">
-        <v>144</v>
+        <v>223</v>
       </c>
     </row>
     <row r="165" spans="1:2" ht="15.5">
@@ -2627,7 +2800,7 @@
         <v>14</v>
       </c>
       <c r="B165" s="5" t="s">
-        <v>224</v>
+        <v>142</v>
       </c>
     </row>
     <row r="166" spans="1:2" ht="15.5">
@@ -2635,7 +2808,7 @@
         <v>14</v>
       </c>
       <c r="B166" s="5" t="s">
-        <v>143</v>
+        <v>224</v>
       </c>
     </row>
     <row r="167" spans="1:2" ht="15.5">
@@ -2683,7 +2856,7 @@
         <v>14</v>
       </c>
       <c r="B172" s="5" t="s">
-        <v>230</v>
+        <v>153</v>
       </c>
     </row>
     <row r="173" spans="1:2" ht="15.5">
@@ -2691,7 +2864,7 @@
         <v>14</v>
       </c>
       <c r="B173" s="5" t="s">
-        <v>154</v>
+        <v>147</v>
       </c>
     </row>
     <row r="174" spans="1:2" ht="15.5">
@@ -2699,7 +2872,7 @@
         <v>14</v>
       </c>
       <c r="B174" s="5" t="s">
-        <v>148</v>
+        <v>230</v>
       </c>
     </row>
     <row r="175" spans="1:2" ht="15.5">
@@ -2707,7 +2880,7 @@
         <v>14</v>
       </c>
       <c r="B175" s="5" t="s">
-        <v>231</v>
+        <v>151</v>
       </c>
     </row>
     <row r="176" spans="1:2" ht="15.5">
@@ -2723,7 +2896,7 @@
         <v>14</v>
       </c>
       <c r="B177" s="5" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
     </row>
     <row r="178" spans="1:2" ht="15.5">
@@ -2731,7 +2904,7 @@
         <v>14</v>
       </c>
       <c r="B178" s="5" t="s">
-        <v>155</v>
+        <v>231</v>
       </c>
     </row>
     <row r="179" spans="1:2" ht="15.5">
@@ -2827,7 +3000,7 @@
         <v>14</v>
       </c>
       <c r="B190" s="5" t="s">
-        <v>243</v>
+        <v>157</v>
       </c>
     </row>
     <row r="191" spans="1:2" ht="15.5">
@@ -2851,7 +3024,7 @@
         <v>14</v>
       </c>
       <c r="B193" s="5" t="s">
-        <v>160</v>
+        <v>243</v>
       </c>
     </row>
     <row r="194" spans="1:2" ht="15.5">
@@ -2883,7 +3056,7 @@
         <v>14</v>
       </c>
       <c r="B197" s="5" t="s">
-        <v>247</v>
+        <v>162</v>
       </c>
     </row>
     <row r="198" spans="1:2" ht="15.5">
@@ -2891,7 +3064,7 @@
         <v>14</v>
       </c>
       <c r="B198" s="5" t="s">
-        <v>163</v>
+        <v>247</v>
       </c>
     </row>
     <row r="199" spans="1:2" ht="15.5">
@@ -2899,7 +3072,7 @@
         <v>14</v>
       </c>
       <c r="B199" s="5" t="s">
-        <v>248</v>
+        <v>164</v>
       </c>
     </row>
     <row r="200" spans="1:2" ht="15.5">
@@ -2907,7 +3080,7 @@
         <v>14</v>
       </c>
       <c r="B200" s="5" t="s">
-        <v>165</v>
+        <v>248</v>
       </c>
     </row>
     <row r="201" spans="1:2" ht="15.5">
@@ -2963,7 +3136,7 @@
         <v>14</v>
       </c>
       <c r="B207" s="5" t="s">
-        <v>255</v>
+        <v>171</v>
       </c>
     </row>
     <row r="208" spans="1:2" ht="15.5">
@@ -2971,7 +3144,7 @@
         <v>14</v>
       </c>
       <c r="B208" s="5" t="s">
-        <v>172</v>
+        <v>255</v>
       </c>
     </row>
     <row r="209" spans="1:2" ht="15.5">
@@ -2995,7 +3168,7 @@
         <v>14</v>
       </c>
       <c r="B211" s="5" t="s">
-        <v>258</v>
+        <v>169</v>
       </c>
     </row>
     <row r="212" spans="1:2" ht="15.5">
@@ -3003,7 +3176,7 @@
         <v>14</v>
       </c>
       <c r="B212" s="5" t="s">
-        <v>170</v>
+        <v>258</v>
       </c>
     </row>
     <row r="213" spans="1:2" ht="15.5">
@@ -3035,7 +3208,7 @@
         <v>14</v>
       </c>
       <c r="B216" s="5" t="s">
-        <v>262</v>
+        <v>168</v>
       </c>
     </row>
     <row r="217" spans="1:2" ht="15.5">
@@ -3043,7 +3216,7 @@
         <v>14</v>
       </c>
       <c r="B217" s="5" t="s">
-        <v>169</v>
+        <v>262</v>
       </c>
     </row>
     <row r="218" spans="1:2" ht="15.5">
@@ -3064,10 +3237,10 @@
     </row>
     <row r="220" spans="1:2" ht="15.5">
       <c r="A220" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B220" s="5" t="s">
-        <v>265</v>
+        <v>84</v>
       </c>
     </row>
     <row r="221" spans="1:2" ht="15.5">
@@ -3780,14 +3953,6 @@
       </c>
       <c r="B309" s="5" t="s">
         <v>173</v>
-      </c>
-    </row>
-    <row r="310" spans="1:2" ht="15.5">
-      <c r="A310" t="s">
-        <v>15</v>
-      </c>
-      <c r="B310" s="5" t="s">
-        <v>174</v>
       </c>
     </row>
   </sheetData>
@@ -3797,2674 +3962,6 @@
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L2:L1048576" xr:uid="{65EC56E6-3255-4BA7-8D1C-8F79B7E5B18C}">
       <formula1>"Active, Inactive, Discontinued"</formula1>
-    </dataValidation>
-  </dataValidations>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{140D0306-11E7-4EAC-BF2E-8F375561574C}">
-  <dimension ref="A1:C241"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
-  <cols>
-    <col min="1" max="1" width="25.6328125" customWidth="1"/>
-    <col min="2" max="2" width="50.6328125" customWidth="1"/>
-    <col min="3" max="3" width="23.81640625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3">
-      <c r="A1" t="s">
-        <v>268</v>
-      </c>
-      <c r="B1" t="s">
-        <v>269</v>
-      </c>
-      <c r="C1" t="s">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" ht="15.5">
-      <c r="A2" t="s">
-        <v>14</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>85</v>
-      </c>
-      <c r="C2">
-        <v>120776</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" ht="15.5">
-      <c r="A3" t="s">
-        <v>14</v>
-      </c>
-      <c r="B3" s="5" t="s">
-        <v>86</v>
-      </c>
-      <c r="C3">
-        <v>120776</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" ht="15.5">
-      <c r="A4" t="s">
-        <v>14</v>
-      </c>
-      <c r="B4" s="5" t="s">
-        <v>87</v>
-      </c>
-      <c r="C4">
-        <v>120776</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" ht="15.5">
-      <c r="A5" t="s">
-        <v>14</v>
-      </c>
-      <c r="B5" s="5" t="s">
-        <v>175</v>
-      </c>
-      <c r="C5">
-        <v>120776</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" ht="15.5">
-      <c r="A6" t="s">
-        <v>14</v>
-      </c>
-      <c r="B6" s="5" t="s">
-        <v>176</v>
-      </c>
-      <c r="C6">
-        <v>120776</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" ht="15.5">
-      <c r="A7" t="s">
-        <v>14</v>
-      </c>
-      <c r="B7" s="5" t="s">
-        <v>88</v>
-      </c>
-      <c r="C7">
-        <v>120776</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" ht="15.5">
-      <c r="A8" t="s">
-        <v>14</v>
-      </c>
-      <c r="B8" s="5" t="s">
-        <v>177</v>
-      </c>
-      <c r="C8">
-        <v>120776</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" ht="15.5">
-      <c r="A9" t="s">
-        <v>14</v>
-      </c>
-      <c r="B9" s="5" t="s">
-        <v>178</v>
-      </c>
-      <c r="C9">
-        <v>120776</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" ht="15.5">
-      <c r="A10" t="s">
-        <v>14</v>
-      </c>
-      <c r="B10" s="5" t="s">
-        <v>89</v>
-      </c>
-      <c r="C10">
-        <v>120776</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" ht="15.5">
-      <c r="A11" t="s">
-        <v>14</v>
-      </c>
-      <c r="B11" s="5" t="s">
-        <v>90</v>
-      </c>
-      <c r="C11">
-        <v>120776</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" ht="15.5">
-      <c r="A12" t="s">
-        <v>14</v>
-      </c>
-      <c r="B12" s="5" t="s">
-        <v>91</v>
-      </c>
-      <c r="C12">
-        <v>120776</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" ht="15.5">
-      <c r="A13" t="s">
-        <v>14</v>
-      </c>
-      <c r="B13" s="5" t="s">
-        <v>179</v>
-      </c>
-      <c r="C13">
-        <v>120776</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" ht="15.5">
-      <c r="A14" t="s">
-        <v>14</v>
-      </c>
-      <c r="B14" s="5" t="s">
-        <v>180</v>
-      </c>
-      <c r="C14">
-        <v>120776</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" ht="15.5">
-      <c r="A15" t="s">
-        <v>14</v>
-      </c>
-      <c r="B15" s="5" t="s">
-        <v>181</v>
-      </c>
-      <c r="C15">
-        <v>120776</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" ht="15.5">
-      <c r="A16" t="s">
-        <v>14</v>
-      </c>
-      <c r="B16" s="5" t="s">
-        <v>182</v>
-      </c>
-      <c r="C16">
-        <v>120776</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" ht="15.5">
-      <c r="A17" t="s">
-        <v>14</v>
-      </c>
-      <c r="B17" s="5" t="s">
-        <v>183</v>
-      </c>
-      <c r="C17">
-        <v>120776</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" ht="15.5">
-      <c r="A18" t="s">
-        <v>14</v>
-      </c>
-      <c r="B18" s="5" t="s">
-        <v>184</v>
-      </c>
-      <c r="C18">
-        <v>120776</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" ht="15.5">
-      <c r="A19" t="s">
-        <v>14</v>
-      </c>
-      <c r="B19" s="5" t="s">
-        <v>185</v>
-      </c>
-      <c r="C19">
-        <v>120776</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" ht="15.5">
-      <c r="A20" t="s">
-        <v>14</v>
-      </c>
-      <c r="B20" s="5" t="s">
-        <v>186</v>
-      </c>
-      <c r="C20">
-        <v>120776</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" ht="15.5">
-      <c r="A21" t="s">
-        <v>14</v>
-      </c>
-      <c r="B21" s="5" t="s">
-        <v>187</v>
-      </c>
-      <c r="C21">
-        <v>120776</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" ht="15.5">
-      <c r="A22" t="s">
-        <v>14</v>
-      </c>
-      <c r="B22" s="5" t="s">
-        <v>188</v>
-      </c>
-      <c r="C22">
-        <v>120776</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" ht="15.5">
-      <c r="A23" t="s">
-        <v>14</v>
-      </c>
-      <c r="B23" s="5" t="s">
-        <v>101</v>
-      </c>
-      <c r="C23">
-        <v>120776</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" ht="15.5">
-      <c r="A24" t="s">
-        <v>14</v>
-      </c>
-      <c r="B24" s="5" t="s">
-        <v>102</v>
-      </c>
-      <c r="C24">
-        <v>120776</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" ht="15.5">
-      <c r="A25" t="s">
-        <v>14</v>
-      </c>
-      <c r="B25" s="5" t="s">
-        <v>189</v>
-      </c>
-      <c r="C25">
-        <v>120776</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" ht="15.5">
-      <c r="A26" t="s">
-        <v>14</v>
-      </c>
-      <c r="B26" s="5" t="s">
-        <v>190</v>
-      </c>
-      <c r="C26">
-        <v>120776</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" ht="15.5">
-      <c r="A27" t="s">
-        <v>14</v>
-      </c>
-      <c r="B27" s="5" t="s">
-        <v>191</v>
-      </c>
-      <c r="C27">
-        <v>120776</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" ht="15.5">
-      <c r="A28" t="s">
-        <v>14</v>
-      </c>
-      <c r="B28" s="5" t="s">
-        <v>98</v>
-      </c>
-      <c r="C28">
-        <v>120776</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" ht="15.5">
-      <c r="A29" t="s">
-        <v>14</v>
-      </c>
-      <c r="B29" s="5" t="s">
-        <v>99</v>
-      </c>
-      <c r="C29">
-        <v>120776</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" ht="15.5">
-      <c r="A30" t="s">
-        <v>14</v>
-      </c>
-      <c r="B30" s="5" t="s">
-        <v>192</v>
-      </c>
-      <c r="C30">
-        <v>120776</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" ht="15.5">
-      <c r="A31" t="s">
-        <v>14</v>
-      </c>
-      <c r="B31" s="5" t="s">
-        <v>103</v>
-      </c>
-      <c r="C31">
-        <v>120776</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" ht="15.5">
-      <c r="A32" t="s">
-        <v>14</v>
-      </c>
-      <c r="B32" s="5" t="s">
-        <v>193</v>
-      </c>
-      <c r="C32">
-        <v>120776</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" ht="15.5">
-      <c r="A33" t="s">
-        <v>14</v>
-      </c>
-      <c r="B33" s="5" t="s">
-        <v>194</v>
-      </c>
-      <c r="C33">
-        <v>120776</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" ht="15.5">
-      <c r="A34" t="s">
-        <v>14</v>
-      </c>
-      <c r="B34" s="5" t="s">
-        <v>195</v>
-      </c>
-      <c r="C34">
-        <v>120776</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" ht="15.5">
-      <c r="A35" t="s">
-        <v>14</v>
-      </c>
-      <c r="B35" s="5" t="s">
-        <v>196</v>
-      </c>
-      <c r="C35">
-        <v>120776</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" ht="15.5">
-      <c r="A36" t="s">
-        <v>14</v>
-      </c>
-      <c r="B36" s="5" t="s">
-        <v>197</v>
-      </c>
-      <c r="C36">
-        <v>120776</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" ht="15.5">
-      <c r="A37" t="s">
-        <v>14</v>
-      </c>
-      <c r="B37" s="5" t="s">
-        <v>198</v>
-      </c>
-      <c r="C37">
-        <v>120776</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" ht="15.5">
-      <c r="A38" t="s">
-        <v>14</v>
-      </c>
-      <c r="B38" s="5" t="s">
-        <v>199</v>
-      </c>
-      <c r="C38">
-        <v>120776</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" ht="15.5">
-      <c r="A39" t="s">
-        <v>14</v>
-      </c>
-      <c r="B39" s="5" t="s">
-        <v>139</v>
-      </c>
-      <c r="C39">
-        <v>120776</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3" ht="15.5">
-      <c r="A40" t="s">
-        <v>14</v>
-      </c>
-      <c r="B40" s="5" t="s">
-        <v>104</v>
-      </c>
-      <c r="C40">
-        <v>120776</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" ht="15.5">
-      <c r="A41" t="s">
-        <v>14</v>
-      </c>
-      <c r="B41" s="5" t="s">
-        <v>105</v>
-      </c>
-      <c r="C41">
-        <v>120776</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" ht="15.5">
-      <c r="A42" t="s">
-        <v>14</v>
-      </c>
-      <c r="B42" s="5" t="s">
-        <v>106</v>
-      </c>
-      <c r="C42">
-        <v>120776</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3" ht="15.5">
-      <c r="A43" t="s">
-        <v>14</v>
-      </c>
-      <c r="B43" s="5" t="s">
-        <v>200</v>
-      </c>
-      <c r="C43">
-        <v>120776</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3" ht="15.5">
-      <c r="A44" t="s">
-        <v>14</v>
-      </c>
-      <c r="B44" s="5" t="s">
-        <v>201</v>
-      </c>
-      <c r="C44">
-        <v>120776</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3" ht="15.5">
-      <c r="A45" t="s">
-        <v>14</v>
-      </c>
-      <c r="B45" s="5" t="s">
-        <v>110</v>
-      </c>
-      <c r="C45">
-        <v>120776</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3" ht="15.5">
-      <c r="A46" t="s">
-        <v>14</v>
-      </c>
-      <c r="B46" s="5" t="s">
-        <v>202</v>
-      </c>
-      <c r="C46">
-        <v>120776</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3" ht="15.5">
-      <c r="A47" t="s">
-        <v>14</v>
-      </c>
-      <c r="B47" s="5" t="s">
-        <v>203</v>
-      </c>
-      <c r="C47">
-        <v>120776</v>
-      </c>
-    </row>
-    <row r="48" spans="1:3" ht="15.5">
-      <c r="A48" t="s">
-        <v>14</v>
-      </c>
-      <c r="B48" s="5" t="s">
-        <v>204</v>
-      </c>
-      <c r="C48">
-        <v>120776</v>
-      </c>
-    </row>
-    <row r="49" spans="1:3" ht="15.5">
-      <c r="A49" t="s">
-        <v>14</v>
-      </c>
-      <c r="B49" s="5" t="s">
-        <v>205</v>
-      </c>
-      <c r="C49">
-        <v>120776</v>
-      </c>
-    </row>
-    <row r="50" spans="1:3" ht="15.5">
-      <c r="A50" t="s">
-        <v>14</v>
-      </c>
-      <c r="B50" s="5" t="s">
-        <v>206</v>
-      </c>
-      <c r="C50">
-        <v>120776</v>
-      </c>
-    </row>
-    <row r="51" spans="1:3" ht="15.5">
-      <c r="A51" t="s">
-        <v>14</v>
-      </c>
-      <c r="B51" s="5" t="s">
-        <v>207</v>
-      </c>
-      <c r="C51">
-        <v>120776</v>
-      </c>
-    </row>
-    <row r="52" spans="1:3" ht="15.5">
-      <c r="A52" t="s">
-        <v>14</v>
-      </c>
-      <c r="B52" s="5" t="s">
-        <v>119</v>
-      </c>
-      <c r="C52">
-        <v>120776</v>
-      </c>
-    </row>
-    <row r="53" spans="1:3" ht="15.5">
-      <c r="A53" t="s">
-        <v>14</v>
-      </c>
-      <c r="B53" s="5" t="s">
-        <v>111</v>
-      </c>
-      <c r="C53">
-        <v>120776</v>
-      </c>
-    </row>
-    <row r="54" spans="1:3" ht="15.5">
-      <c r="A54" t="s">
-        <v>14</v>
-      </c>
-      <c r="B54" s="5" t="s">
-        <v>128</v>
-      </c>
-      <c r="C54">
-        <v>120776</v>
-      </c>
-    </row>
-    <row r="55" spans="1:3" ht="15.5">
-      <c r="A55" t="s">
-        <v>14</v>
-      </c>
-      <c r="B55" s="5" t="s">
-        <v>129</v>
-      </c>
-      <c r="C55">
-        <v>120776</v>
-      </c>
-    </row>
-    <row r="56" spans="1:3" ht="15.5">
-      <c r="A56" t="s">
-        <v>14</v>
-      </c>
-      <c r="B56" s="5" t="s">
-        <v>112</v>
-      </c>
-      <c r="C56">
-        <v>120776</v>
-      </c>
-    </row>
-    <row r="57" spans="1:3" ht="15.5">
-      <c r="A57" t="s">
-        <v>14</v>
-      </c>
-      <c r="B57" s="5" t="s">
-        <v>208</v>
-      </c>
-      <c r="C57">
-        <v>120776</v>
-      </c>
-    </row>
-    <row r="58" spans="1:3" ht="15.5">
-      <c r="A58" t="s">
-        <v>14</v>
-      </c>
-      <c r="B58" s="5" t="s">
-        <v>150</v>
-      </c>
-      <c r="C58">
-        <v>120776</v>
-      </c>
-    </row>
-    <row r="59" spans="1:3" ht="15.5">
-      <c r="A59" t="s">
-        <v>14</v>
-      </c>
-      <c r="B59" s="5" t="s">
-        <v>151</v>
-      </c>
-      <c r="C59">
-        <v>120776</v>
-      </c>
-    </row>
-    <row r="60" spans="1:3" ht="15.5">
-      <c r="A60" t="s">
-        <v>14</v>
-      </c>
-      <c r="B60" s="5" t="s">
-        <v>113</v>
-      </c>
-      <c r="C60">
-        <v>120776</v>
-      </c>
-    </row>
-    <row r="61" spans="1:3" ht="15.5">
-      <c r="A61" t="s">
-        <v>14</v>
-      </c>
-      <c r="B61" s="5" t="s">
-        <v>209</v>
-      </c>
-      <c r="C61">
-        <v>120776</v>
-      </c>
-    </row>
-    <row r="62" spans="1:3" ht="15.5">
-      <c r="A62" t="s">
-        <v>14</v>
-      </c>
-      <c r="B62" s="5" t="s">
-        <v>210</v>
-      </c>
-      <c r="C62">
-        <v>120776</v>
-      </c>
-    </row>
-    <row r="63" spans="1:3" ht="15.5">
-      <c r="A63" t="s">
-        <v>14</v>
-      </c>
-      <c r="B63" s="5" t="s">
-        <v>114</v>
-      </c>
-      <c r="C63">
-        <v>120776</v>
-      </c>
-    </row>
-    <row r="64" spans="1:3" ht="15.5">
-      <c r="A64" t="s">
-        <v>14</v>
-      </c>
-      <c r="B64" s="5" t="s">
-        <v>135</v>
-      </c>
-      <c r="C64">
-        <v>120776</v>
-      </c>
-    </row>
-    <row r="65" spans="1:3" ht="15.5">
-      <c r="A65" t="s">
-        <v>14</v>
-      </c>
-      <c r="B65" s="5" t="s">
-        <v>211</v>
-      </c>
-      <c r="C65">
-        <v>120776</v>
-      </c>
-    </row>
-    <row r="66" spans="1:3" ht="15.5">
-      <c r="A66" t="s">
-        <v>14</v>
-      </c>
-      <c r="B66" s="5" t="s">
-        <v>115</v>
-      </c>
-      <c r="C66">
-        <v>120776</v>
-      </c>
-    </row>
-    <row r="67" spans="1:3" ht="15.5">
-      <c r="A67" t="s">
-        <v>14</v>
-      </c>
-      <c r="B67" s="5" t="s">
-        <v>212</v>
-      </c>
-      <c r="C67">
-        <v>120776</v>
-      </c>
-    </row>
-    <row r="68" spans="1:3" ht="15.5">
-      <c r="A68" t="s">
-        <v>14</v>
-      </c>
-      <c r="B68" s="5" t="s">
-        <v>132</v>
-      </c>
-      <c r="C68">
-        <v>120776</v>
-      </c>
-    </row>
-    <row r="69" spans="1:3" ht="15.5">
-      <c r="A69" t="s">
-        <v>14</v>
-      </c>
-      <c r="B69" s="5" t="s">
-        <v>118</v>
-      </c>
-      <c r="C69">
-        <v>120776</v>
-      </c>
-    </row>
-    <row r="70" spans="1:3" ht="15.5">
-      <c r="A70" t="s">
-        <v>14</v>
-      </c>
-      <c r="B70" s="5" t="s">
-        <v>213</v>
-      </c>
-      <c r="C70">
-        <v>120776</v>
-      </c>
-    </row>
-    <row r="71" spans="1:3" ht="15.5">
-      <c r="A71" t="s">
-        <v>14</v>
-      </c>
-      <c r="B71" s="5" t="s">
-        <v>116</v>
-      </c>
-      <c r="C71">
-        <v>120776</v>
-      </c>
-    </row>
-    <row r="72" spans="1:3" ht="15.5">
-      <c r="A72" t="s">
-        <v>14</v>
-      </c>
-      <c r="B72" s="5" t="s">
-        <v>117</v>
-      </c>
-      <c r="C72">
-        <v>120776</v>
-      </c>
-    </row>
-    <row r="73" spans="1:3" ht="15.5">
-      <c r="A73" t="s">
-        <v>14</v>
-      </c>
-      <c r="B73" s="5" t="s">
-        <v>120</v>
-      </c>
-      <c r="C73">
-        <v>120776</v>
-      </c>
-    </row>
-    <row r="74" spans="1:3" ht="15.5">
-      <c r="A74" t="s">
-        <v>14</v>
-      </c>
-      <c r="B74" s="5" t="s">
-        <v>121</v>
-      </c>
-      <c r="C74">
-        <v>120776</v>
-      </c>
-    </row>
-    <row r="75" spans="1:3" ht="15.5">
-      <c r="A75" t="s">
-        <v>14</v>
-      </c>
-      <c r="B75" s="5" t="s">
-        <v>214</v>
-      </c>
-      <c r="C75">
-        <v>120776</v>
-      </c>
-    </row>
-    <row r="76" spans="1:3" ht="15.5">
-      <c r="A76" t="s">
-        <v>14</v>
-      </c>
-      <c r="B76" s="5" t="s">
-        <v>122</v>
-      </c>
-      <c r="C76">
-        <v>120776</v>
-      </c>
-    </row>
-    <row r="77" spans="1:3" ht="15.5">
-      <c r="A77" t="s">
-        <v>14</v>
-      </c>
-      <c r="B77" s="5" t="s">
-        <v>123</v>
-      </c>
-      <c r="C77">
-        <v>120776</v>
-      </c>
-    </row>
-    <row r="78" spans="1:3" ht="15.5">
-      <c r="A78" t="s">
-        <v>14</v>
-      </c>
-      <c r="B78" s="5" t="s">
-        <v>215</v>
-      </c>
-      <c r="C78">
-        <v>120776</v>
-      </c>
-    </row>
-    <row r="79" spans="1:3" ht="15.5">
-      <c r="A79" t="s">
-        <v>14</v>
-      </c>
-      <c r="B79" s="5" t="s">
-        <v>124</v>
-      </c>
-      <c r="C79">
-        <v>120776</v>
-      </c>
-    </row>
-    <row r="80" spans="1:3" ht="15.5">
-      <c r="A80" t="s">
-        <v>14</v>
-      </c>
-      <c r="B80" s="5" t="s">
-        <v>133</v>
-      </c>
-      <c r="C80">
-        <v>120776</v>
-      </c>
-    </row>
-    <row r="81" spans="1:3" ht="15.5">
-      <c r="A81" t="s">
-        <v>14</v>
-      </c>
-      <c r="B81" s="5" t="s">
-        <v>125</v>
-      </c>
-      <c r="C81">
-        <v>120776</v>
-      </c>
-    </row>
-    <row r="82" spans="1:3" ht="15.5">
-      <c r="A82" t="s">
-        <v>14</v>
-      </c>
-      <c r="B82" s="5" t="s">
-        <v>216</v>
-      </c>
-      <c r="C82">
-        <v>120776</v>
-      </c>
-    </row>
-    <row r="83" spans="1:3" ht="15.5">
-      <c r="A83" t="s">
-        <v>14</v>
-      </c>
-      <c r="B83" s="5" t="s">
-        <v>137</v>
-      </c>
-      <c r="C83">
-        <v>120776</v>
-      </c>
-    </row>
-    <row r="84" spans="1:3" ht="15.5">
-      <c r="A84" t="s">
-        <v>14</v>
-      </c>
-      <c r="B84" s="5" t="s">
-        <v>138</v>
-      </c>
-      <c r="C84">
-        <v>120776</v>
-      </c>
-    </row>
-    <row r="85" spans="1:3" ht="15.5">
-      <c r="A85" t="s">
-        <v>14</v>
-      </c>
-      <c r="B85" s="5" t="s">
-        <v>217</v>
-      </c>
-      <c r="C85">
-        <v>120776</v>
-      </c>
-    </row>
-    <row r="86" spans="1:3" ht="15.5">
-      <c r="A86" t="s">
-        <v>14</v>
-      </c>
-      <c r="B86" s="5" t="s">
-        <v>218</v>
-      </c>
-      <c r="C86">
-        <v>120776</v>
-      </c>
-    </row>
-    <row r="87" spans="1:3" ht="15.5">
-      <c r="A87" t="s">
-        <v>14</v>
-      </c>
-      <c r="B87" s="5" t="s">
-        <v>219</v>
-      </c>
-      <c r="C87">
-        <v>120776</v>
-      </c>
-    </row>
-    <row r="88" spans="1:3" ht="15.5">
-      <c r="A88" t="s">
-        <v>14</v>
-      </c>
-      <c r="B88" s="5" t="s">
-        <v>220</v>
-      </c>
-      <c r="C88">
-        <v>120776</v>
-      </c>
-    </row>
-    <row r="89" spans="1:3" ht="15.5">
-      <c r="A89" t="s">
-        <v>14</v>
-      </c>
-      <c r="B89" s="5" t="s">
-        <v>140</v>
-      </c>
-      <c r="C89">
-        <v>120776</v>
-      </c>
-    </row>
-    <row r="90" spans="1:3" ht="15.5">
-      <c r="A90" t="s">
-        <v>14</v>
-      </c>
-      <c r="B90" s="5" t="s">
-        <v>221</v>
-      </c>
-      <c r="C90">
-        <v>120776</v>
-      </c>
-    </row>
-    <row r="91" spans="1:3" ht="15.5">
-      <c r="A91" t="s">
-        <v>14</v>
-      </c>
-      <c r="B91" s="5" t="s">
-        <v>222</v>
-      </c>
-      <c r="C91">
-        <v>120776</v>
-      </c>
-    </row>
-    <row r="92" spans="1:3" ht="15.5">
-      <c r="A92" t="s">
-        <v>14</v>
-      </c>
-      <c r="B92" s="5" t="s">
-        <v>223</v>
-      </c>
-      <c r="C92">
-        <v>120776</v>
-      </c>
-    </row>
-    <row r="93" spans="1:3" ht="15.5">
-      <c r="A93" t="s">
-        <v>14</v>
-      </c>
-      <c r="B93" s="5" t="s">
-        <v>142</v>
-      </c>
-      <c r="C93">
-        <v>120776</v>
-      </c>
-    </row>
-    <row r="94" spans="1:3" ht="15.5">
-      <c r="A94" t="s">
-        <v>14</v>
-      </c>
-      <c r="B94" s="5" t="s">
-        <v>144</v>
-      </c>
-      <c r="C94">
-        <v>120776</v>
-      </c>
-    </row>
-    <row r="95" spans="1:3" ht="15.5">
-      <c r="A95" t="s">
-        <v>14</v>
-      </c>
-      <c r="B95" s="5" t="s">
-        <v>224</v>
-      </c>
-      <c r="C95">
-        <v>120776</v>
-      </c>
-    </row>
-    <row r="96" spans="1:3" ht="15.5">
-      <c r="A96" t="s">
-        <v>14</v>
-      </c>
-      <c r="B96" s="5" t="s">
-        <v>143</v>
-      </c>
-      <c r="C96">
-        <v>120776</v>
-      </c>
-    </row>
-    <row r="97" spans="1:3" ht="15.5">
-      <c r="A97" t="s">
-        <v>14</v>
-      </c>
-      <c r="B97" s="5" t="s">
-        <v>225</v>
-      </c>
-      <c r="C97">
-        <v>120776</v>
-      </c>
-    </row>
-    <row r="98" spans="1:3" ht="15.5">
-      <c r="A98" t="s">
-        <v>14</v>
-      </c>
-      <c r="B98" s="5" t="s">
-        <v>226</v>
-      </c>
-      <c r="C98">
-        <v>120776</v>
-      </c>
-    </row>
-    <row r="99" spans="1:3" ht="15.5">
-      <c r="A99" t="s">
-        <v>14</v>
-      </c>
-      <c r="B99" s="5" t="s">
-        <v>227</v>
-      </c>
-      <c r="C99">
-        <v>120776</v>
-      </c>
-    </row>
-    <row r="100" spans="1:3" ht="15.5">
-      <c r="A100" t="s">
-        <v>14</v>
-      </c>
-      <c r="B100" s="5" t="s">
-        <v>228</v>
-      </c>
-      <c r="C100">
-        <v>120776</v>
-      </c>
-    </row>
-    <row r="101" spans="1:3" ht="15.5">
-      <c r="A101" t="s">
-        <v>14</v>
-      </c>
-      <c r="B101" s="5" t="s">
-        <v>229</v>
-      </c>
-      <c r="C101">
-        <v>120776</v>
-      </c>
-    </row>
-    <row r="102" spans="1:3" ht="15.5">
-      <c r="A102" t="s">
-        <v>14</v>
-      </c>
-      <c r="B102" s="5" t="s">
-        <v>230</v>
-      </c>
-      <c r="C102">
-        <v>120776</v>
-      </c>
-    </row>
-    <row r="103" spans="1:3" ht="15.5">
-      <c r="A103" t="s">
-        <v>14</v>
-      </c>
-      <c r="B103" s="5" t="s">
-        <v>154</v>
-      </c>
-      <c r="C103">
-        <v>120776</v>
-      </c>
-    </row>
-    <row r="104" spans="1:3" ht="15.5">
-      <c r="A104" t="s">
-        <v>14</v>
-      </c>
-      <c r="B104" s="5" t="s">
-        <v>148</v>
-      </c>
-      <c r="C104">
-        <v>120776</v>
-      </c>
-    </row>
-    <row r="105" spans="1:3" ht="15.5">
-      <c r="A105" t="s">
-        <v>14</v>
-      </c>
-      <c r="B105" s="5" t="s">
-        <v>231</v>
-      </c>
-      <c r="C105">
-        <v>120776</v>
-      </c>
-    </row>
-    <row r="106" spans="1:3" ht="15.5">
-      <c r="A106" t="s">
-        <v>14</v>
-      </c>
-      <c r="B106" s="5" t="s">
-        <v>152</v>
-      </c>
-      <c r="C106">
-        <v>120776</v>
-      </c>
-    </row>
-    <row r="107" spans="1:3" ht="15.5">
-      <c r="A107" t="s">
-        <v>14</v>
-      </c>
-      <c r="B107" s="5" t="s">
-        <v>153</v>
-      </c>
-      <c r="C107">
-        <v>120776</v>
-      </c>
-    </row>
-    <row r="108" spans="1:3" ht="15.5">
-      <c r="A108" t="s">
-        <v>14</v>
-      </c>
-      <c r="B108" s="5" t="s">
-        <v>155</v>
-      </c>
-      <c r="C108">
-        <v>120776</v>
-      </c>
-    </row>
-    <row r="109" spans="1:3" ht="15.5">
-      <c r="A109" t="s">
-        <v>14</v>
-      </c>
-      <c r="B109" s="5" t="s">
-        <v>232</v>
-      </c>
-      <c r="C109">
-        <v>120776</v>
-      </c>
-    </row>
-    <row r="110" spans="1:3" ht="15.5">
-      <c r="A110" t="s">
-        <v>14</v>
-      </c>
-      <c r="B110" s="5" t="s">
-        <v>233</v>
-      </c>
-      <c r="C110">
-        <v>120776</v>
-      </c>
-    </row>
-    <row r="111" spans="1:3" ht="15.5">
-      <c r="A111" t="s">
-        <v>14</v>
-      </c>
-      <c r="B111" s="5" t="s">
-        <v>234</v>
-      </c>
-      <c r="C111">
-        <v>120776</v>
-      </c>
-    </row>
-    <row r="112" spans="1:3" ht="15.5">
-      <c r="A112" t="s">
-        <v>14</v>
-      </c>
-      <c r="B112" s="5" t="s">
-        <v>235</v>
-      </c>
-      <c r="C112">
-        <v>120776</v>
-      </c>
-    </row>
-    <row r="113" spans="1:3" ht="15.5">
-      <c r="A113" t="s">
-        <v>14</v>
-      </c>
-      <c r="B113" s="5" t="s">
-        <v>236</v>
-      </c>
-      <c r="C113">
-        <v>120776</v>
-      </c>
-    </row>
-    <row r="114" spans="1:3" ht="15.5">
-      <c r="A114" t="s">
-        <v>14</v>
-      </c>
-      <c r="B114" s="5" t="s">
-        <v>237</v>
-      </c>
-      <c r="C114">
-        <v>120776</v>
-      </c>
-    </row>
-    <row r="115" spans="1:3" ht="15.5">
-      <c r="A115" t="s">
-        <v>14</v>
-      </c>
-      <c r="B115" s="5" t="s">
-        <v>238</v>
-      </c>
-      <c r="C115">
-        <v>120776</v>
-      </c>
-    </row>
-    <row r="116" spans="1:3" ht="15.5">
-      <c r="A116" t="s">
-        <v>14</v>
-      </c>
-      <c r="B116" s="5" t="s">
-        <v>239</v>
-      </c>
-      <c r="C116">
-        <v>120776</v>
-      </c>
-    </row>
-    <row r="117" spans="1:3" ht="15.5">
-      <c r="A117" t="s">
-        <v>14</v>
-      </c>
-      <c r="B117" s="5" t="s">
-        <v>240</v>
-      </c>
-      <c r="C117">
-        <v>120776</v>
-      </c>
-    </row>
-    <row r="118" spans="1:3" ht="15.5">
-      <c r="A118" t="s">
-        <v>14</v>
-      </c>
-      <c r="B118" s="5" t="s">
-        <v>241</v>
-      </c>
-      <c r="C118">
-        <v>120776</v>
-      </c>
-    </row>
-    <row r="119" spans="1:3" ht="15.5">
-      <c r="A119" t="s">
-        <v>14</v>
-      </c>
-      <c r="B119" s="5" t="s">
-        <v>242</v>
-      </c>
-      <c r="C119">
-        <v>120776</v>
-      </c>
-    </row>
-    <row r="120" spans="1:3" ht="15.5">
-      <c r="A120" t="s">
-        <v>14</v>
-      </c>
-      <c r="B120" s="5" t="s">
-        <v>243</v>
-      </c>
-      <c r="C120">
-        <v>120776</v>
-      </c>
-    </row>
-    <row r="121" spans="1:3" ht="15.5">
-      <c r="A121" t="s">
-        <v>14</v>
-      </c>
-      <c r="B121" s="5" t="s">
-        <v>158</v>
-      </c>
-      <c r="C121">
-        <v>120776</v>
-      </c>
-    </row>
-    <row r="122" spans="1:3" ht="15.5">
-      <c r="A122" t="s">
-        <v>14</v>
-      </c>
-      <c r="B122" s="5" t="s">
-        <v>159</v>
-      </c>
-      <c r="C122">
-        <v>120776</v>
-      </c>
-    </row>
-    <row r="123" spans="1:3" ht="15.5">
-      <c r="A123" t="s">
-        <v>14</v>
-      </c>
-      <c r="B123" s="5" t="s">
-        <v>160</v>
-      </c>
-      <c r="C123">
-        <v>120776</v>
-      </c>
-    </row>
-    <row r="124" spans="1:3" ht="15.5">
-      <c r="A124" t="s">
-        <v>14</v>
-      </c>
-      <c r="B124" s="5" t="s">
-        <v>244</v>
-      </c>
-      <c r="C124">
-        <v>120776</v>
-      </c>
-    </row>
-    <row r="125" spans="1:3" ht="15.5">
-      <c r="A125" t="s">
-        <v>14</v>
-      </c>
-      <c r="B125" s="5" t="s">
-        <v>245</v>
-      </c>
-      <c r="C125">
-        <v>120776</v>
-      </c>
-    </row>
-    <row r="126" spans="1:3" ht="15.5">
-      <c r="A126" t="s">
-        <v>14</v>
-      </c>
-      <c r="B126" s="5" t="s">
-        <v>246</v>
-      </c>
-      <c r="C126">
-        <v>120776</v>
-      </c>
-    </row>
-    <row r="127" spans="1:3" ht="15.5">
-      <c r="A127" t="s">
-        <v>14</v>
-      </c>
-      <c r="B127" s="5" t="s">
-        <v>247</v>
-      </c>
-      <c r="C127">
-        <v>120776</v>
-      </c>
-    </row>
-    <row r="128" spans="1:3" ht="15.5">
-      <c r="A128" t="s">
-        <v>14</v>
-      </c>
-      <c r="B128" s="5" t="s">
-        <v>163</v>
-      </c>
-      <c r="C128">
-        <v>120776</v>
-      </c>
-    </row>
-    <row r="129" spans="1:3" ht="15.5">
-      <c r="A129" t="s">
-        <v>14</v>
-      </c>
-      <c r="B129" s="5" t="s">
-        <v>248</v>
-      </c>
-      <c r="C129">
-        <v>120776</v>
-      </c>
-    </row>
-    <row r="130" spans="1:3" ht="15.5">
-      <c r="A130" t="s">
-        <v>14</v>
-      </c>
-      <c r="B130" s="5" t="s">
-        <v>165</v>
-      </c>
-      <c r="C130">
-        <v>120776</v>
-      </c>
-    </row>
-    <row r="131" spans="1:3" ht="15.5">
-      <c r="A131" t="s">
-        <v>14</v>
-      </c>
-      <c r="B131" s="5" t="s">
-        <v>249</v>
-      </c>
-      <c r="C131">
-        <v>120776</v>
-      </c>
-    </row>
-    <row r="132" spans="1:3" ht="15.5">
-      <c r="A132" t="s">
-        <v>14</v>
-      </c>
-      <c r="B132" s="5" t="s">
-        <v>250</v>
-      </c>
-      <c r="C132">
-        <v>120776</v>
-      </c>
-    </row>
-    <row r="133" spans="1:3" ht="15.5">
-      <c r="A133" t="s">
-        <v>14</v>
-      </c>
-      <c r="B133" s="5" t="s">
-        <v>251</v>
-      </c>
-      <c r="C133">
-        <v>120776</v>
-      </c>
-    </row>
-    <row r="134" spans="1:3" ht="15.5">
-      <c r="A134" t="s">
-        <v>14</v>
-      </c>
-      <c r="B134" s="5" t="s">
-        <v>252</v>
-      </c>
-      <c r="C134">
-        <v>120776</v>
-      </c>
-    </row>
-    <row r="135" spans="1:3" ht="15.5">
-      <c r="A135" t="s">
-        <v>14</v>
-      </c>
-      <c r="B135" s="5" t="s">
-        <v>253</v>
-      </c>
-      <c r="C135">
-        <v>120776</v>
-      </c>
-    </row>
-    <row r="136" spans="1:3" ht="15.5">
-      <c r="A136" t="s">
-        <v>14</v>
-      </c>
-      <c r="B136" s="5" t="s">
-        <v>254</v>
-      </c>
-      <c r="C136">
-        <v>120776</v>
-      </c>
-    </row>
-    <row r="137" spans="1:3" ht="15.5">
-      <c r="A137" t="s">
-        <v>14</v>
-      </c>
-      <c r="B137" s="5" t="s">
-        <v>255</v>
-      </c>
-      <c r="C137">
-        <v>120776</v>
-      </c>
-    </row>
-    <row r="138" spans="1:3" ht="15.5">
-      <c r="A138" t="s">
-        <v>14</v>
-      </c>
-      <c r="B138" s="5" t="s">
-        <v>172</v>
-      </c>
-      <c r="C138">
-        <v>120776</v>
-      </c>
-    </row>
-    <row r="139" spans="1:3" ht="15.5">
-      <c r="A139" t="s">
-        <v>14</v>
-      </c>
-      <c r="B139" s="5" t="s">
-        <v>256</v>
-      </c>
-      <c r="C139">
-        <v>120776</v>
-      </c>
-    </row>
-    <row r="140" spans="1:3" ht="15.5">
-      <c r="A140" t="s">
-        <v>14</v>
-      </c>
-      <c r="B140" s="5" t="s">
-        <v>257</v>
-      </c>
-      <c r="C140">
-        <v>120776</v>
-      </c>
-    </row>
-    <row r="141" spans="1:3" ht="15.5">
-      <c r="A141" t="s">
-        <v>14</v>
-      </c>
-      <c r="B141" s="5" t="s">
-        <v>258</v>
-      </c>
-      <c r="C141">
-        <v>120776</v>
-      </c>
-    </row>
-    <row r="142" spans="1:3" ht="15.5">
-      <c r="A142" t="s">
-        <v>14</v>
-      </c>
-      <c r="B142" s="5" t="s">
-        <v>170</v>
-      </c>
-      <c r="C142">
-        <v>120776</v>
-      </c>
-    </row>
-    <row r="143" spans="1:3" ht="15.5">
-      <c r="A143" t="s">
-        <v>14</v>
-      </c>
-      <c r="B143" s="5" t="s">
-        <v>259</v>
-      </c>
-      <c r="C143">
-        <v>120776</v>
-      </c>
-    </row>
-    <row r="144" spans="1:3" ht="15.5">
-      <c r="A144" t="s">
-        <v>14</v>
-      </c>
-      <c r="B144" s="5" t="s">
-        <v>260</v>
-      </c>
-      <c r="C144">
-        <v>120776</v>
-      </c>
-    </row>
-    <row r="145" spans="1:3" ht="15.5">
-      <c r="A145" t="s">
-        <v>14</v>
-      </c>
-      <c r="B145" s="5" t="s">
-        <v>261</v>
-      </c>
-      <c r="C145">
-        <v>120776</v>
-      </c>
-    </row>
-    <row r="146" spans="1:3" ht="15.5">
-      <c r="A146" t="s">
-        <v>14</v>
-      </c>
-      <c r="B146" s="5" t="s">
-        <v>262</v>
-      </c>
-      <c r="C146">
-        <v>120776</v>
-      </c>
-    </row>
-    <row r="147" spans="1:3" ht="15.5">
-      <c r="A147" t="s">
-        <v>14</v>
-      </c>
-      <c r="B147" s="5" t="s">
-        <v>169</v>
-      </c>
-      <c r="C147">
-        <v>120776</v>
-      </c>
-    </row>
-    <row r="148" spans="1:3" ht="15.5">
-      <c r="A148" t="s">
-        <v>14</v>
-      </c>
-      <c r="B148" s="5" t="s">
-        <v>263</v>
-      </c>
-      <c r="C148">
-        <v>120776</v>
-      </c>
-    </row>
-    <row r="149" spans="1:3" ht="15.5">
-      <c r="A149" t="s">
-        <v>14</v>
-      </c>
-      <c r="B149" s="5" t="s">
-        <v>264</v>
-      </c>
-      <c r="C149">
-        <v>120776</v>
-      </c>
-    </row>
-    <row r="150" spans="1:3" ht="15.5">
-      <c r="A150" t="s">
-        <v>14</v>
-      </c>
-      <c r="B150" s="5" t="s">
-        <v>265</v>
-      </c>
-      <c r="C150">
-        <v>120776</v>
-      </c>
-    </row>
-    <row r="151" spans="1:3" ht="15.5">
-      <c r="B151" s="5"/>
-    </row>
-    <row r="152" spans="1:3" ht="15.5">
-      <c r="A152" t="s">
-        <v>15</v>
-      </c>
-      <c r="B152" s="5" t="s">
-        <v>85</v>
-      </c>
-      <c r="C152">
-        <v>120775</v>
-      </c>
-    </row>
-    <row r="153" spans="1:3" ht="15.5">
-      <c r="A153" t="s">
-        <v>15</v>
-      </c>
-      <c r="B153" s="5" t="s">
-        <v>86</v>
-      </c>
-      <c r="C153">
-        <v>120775</v>
-      </c>
-    </row>
-    <row r="154" spans="1:3" ht="15.5">
-      <c r="A154" t="s">
-        <v>15</v>
-      </c>
-      <c r="B154" s="5" t="s">
-        <v>87</v>
-      </c>
-      <c r="C154">
-        <v>120775</v>
-      </c>
-    </row>
-    <row r="155" spans="1:3" ht="15.5">
-      <c r="A155" t="s">
-        <v>15</v>
-      </c>
-      <c r="B155" s="5" t="s">
-        <v>88</v>
-      </c>
-      <c r="C155">
-        <v>120775</v>
-      </c>
-    </row>
-    <row r="156" spans="1:3" ht="15.5">
-      <c r="A156" t="s">
-        <v>15</v>
-      </c>
-      <c r="B156" s="5" t="s">
-        <v>89</v>
-      </c>
-      <c r="C156">
-        <v>120775</v>
-      </c>
-    </row>
-    <row r="157" spans="1:3" ht="15.5">
-      <c r="A157" t="s">
-        <v>15</v>
-      </c>
-      <c r="B157" s="5" t="s">
-        <v>90</v>
-      </c>
-      <c r="C157">
-        <v>120775</v>
-      </c>
-    </row>
-    <row r="158" spans="1:3" ht="15.5">
-      <c r="A158" t="s">
-        <v>15</v>
-      </c>
-      <c r="B158" s="5" t="s">
-        <v>91</v>
-      </c>
-      <c r="C158">
-        <v>120775</v>
-      </c>
-    </row>
-    <row r="159" spans="1:3" ht="15.5">
-      <c r="A159" t="s">
-        <v>15</v>
-      </c>
-      <c r="B159" s="5" t="s">
-        <v>92</v>
-      </c>
-      <c r="C159">
-        <v>120775</v>
-      </c>
-    </row>
-    <row r="160" spans="1:3" ht="15.5">
-      <c r="A160" t="s">
-        <v>15</v>
-      </c>
-      <c r="B160" s="5" t="s">
-        <v>93</v>
-      </c>
-      <c r="C160">
-        <v>120775</v>
-      </c>
-    </row>
-    <row r="161" spans="1:3" ht="15.5">
-      <c r="A161" t="s">
-        <v>15</v>
-      </c>
-      <c r="B161" s="5" t="s">
-        <v>94</v>
-      </c>
-      <c r="C161">
-        <v>120775</v>
-      </c>
-    </row>
-    <row r="162" spans="1:3" ht="15.5">
-      <c r="A162" t="s">
-        <v>15</v>
-      </c>
-      <c r="B162" s="5" t="s">
-        <v>95</v>
-      </c>
-      <c r="C162">
-        <v>120775</v>
-      </c>
-    </row>
-    <row r="163" spans="1:3" ht="15.5">
-      <c r="A163" t="s">
-        <v>15</v>
-      </c>
-      <c r="B163" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="C163">
-        <v>120775</v>
-      </c>
-    </row>
-    <row r="164" spans="1:3" ht="15.5">
-      <c r="A164" t="s">
-        <v>15</v>
-      </c>
-      <c r="B164" s="5" t="s">
-        <v>97</v>
-      </c>
-      <c r="C164">
-        <v>120775</v>
-      </c>
-    </row>
-    <row r="165" spans="1:3" ht="15.5">
-      <c r="A165" t="s">
-        <v>15</v>
-      </c>
-      <c r="B165" s="5" t="s">
-        <v>98</v>
-      </c>
-      <c r="C165">
-        <v>120775</v>
-      </c>
-    </row>
-    <row r="166" spans="1:3" ht="15.5">
-      <c r="A166" t="s">
-        <v>15</v>
-      </c>
-      <c r="B166" s="5" t="s">
-        <v>99</v>
-      </c>
-      <c r="C166">
-        <v>120775</v>
-      </c>
-    </row>
-    <row r="167" spans="1:3" ht="15.5">
-      <c r="A167" t="s">
-        <v>15</v>
-      </c>
-      <c r="B167" s="5" t="s">
-        <v>100</v>
-      </c>
-      <c r="C167">
-        <v>120775</v>
-      </c>
-    </row>
-    <row r="168" spans="1:3" ht="15.5">
-      <c r="A168" t="s">
-        <v>15</v>
-      </c>
-      <c r="B168" s="5" t="s">
-        <v>101</v>
-      </c>
-      <c r="C168">
-        <v>120775</v>
-      </c>
-    </row>
-    <row r="169" spans="1:3" ht="15.5">
-      <c r="A169" t="s">
-        <v>15</v>
-      </c>
-      <c r="B169" s="5" t="s">
-        <v>102</v>
-      </c>
-      <c r="C169">
-        <v>120775</v>
-      </c>
-    </row>
-    <row r="170" spans="1:3" ht="15.5">
-      <c r="A170" t="s">
-        <v>15</v>
-      </c>
-      <c r="B170" s="5" t="s">
-        <v>103</v>
-      </c>
-      <c r="C170">
-        <v>120775</v>
-      </c>
-    </row>
-    <row r="171" spans="1:3" ht="15.5">
-      <c r="A171" t="s">
-        <v>15</v>
-      </c>
-      <c r="B171" s="5" t="s">
-        <v>104</v>
-      </c>
-      <c r="C171">
-        <v>120775</v>
-      </c>
-    </row>
-    <row r="172" spans="1:3" ht="15.5">
-      <c r="A172" t="s">
-        <v>15</v>
-      </c>
-      <c r="B172" s="5" t="s">
-        <v>105</v>
-      </c>
-      <c r="C172">
-        <v>120775</v>
-      </c>
-    </row>
-    <row r="173" spans="1:3" ht="15.5">
-      <c r="A173" t="s">
-        <v>15</v>
-      </c>
-      <c r="B173" s="5" t="s">
-        <v>106</v>
-      </c>
-      <c r="C173">
-        <v>120775</v>
-      </c>
-    </row>
-    <row r="174" spans="1:3" ht="15.5">
-      <c r="A174" t="s">
-        <v>15</v>
-      </c>
-      <c r="B174" s="5" t="s">
-        <v>107</v>
-      </c>
-      <c r="C174">
-        <v>120775</v>
-      </c>
-    </row>
-    <row r="175" spans="1:3" ht="15.5">
-      <c r="A175" t="s">
-        <v>15</v>
-      </c>
-      <c r="B175" s="5" t="s">
-        <v>108</v>
-      </c>
-      <c r="C175">
-        <v>120775</v>
-      </c>
-    </row>
-    <row r="176" spans="1:3" ht="15.5">
-      <c r="A176" t="s">
-        <v>15</v>
-      </c>
-      <c r="B176" s="5" t="s">
-        <v>109</v>
-      </c>
-      <c r="C176">
-        <v>120775</v>
-      </c>
-    </row>
-    <row r="177" spans="1:3" ht="15.5">
-      <c r="A177" t="s">
-        <v>15</v>
-      </c>
-      <c r="B177" s="5" t="s">
-        <v>110</v>
-      </c>
-      <c r="C177">
-        <v>120775</v>
-      </c>
-    </row>
-    <row r="178" spans="1:3" ht="15.5">
-      <c r="A178" t="s">
-        <v>15</v>
-      </c>
-      <c r="B178" s="5" t="s">
-        <v>111</v>
-      </c>
-      <c r="C178">
-        <v>120775</v>
-      </c>
-    </row>
-    <row r="179" spans="1:3" ht="15.5">
-      <c r="A179" t="s">
-        <v>15</v>
-      </c>
-      <c r="B179" s="5" t="s">
-        <v>112</v>
-      </c>
-      <c r="C179">
-        <v>120775</v>
-      </c>
-    </row>
-    <row r="180" spans="1:3" ht="15.5">
-      <c r="A180" t="s">
-        <v>15</v>
-      </c>
-      <c r="B180" s="5" t="s">
-        <v>113</v>
-      </c>
-      <c r="C180">
-        <v>120775</v>
-      </c>
-    </row>
-    <row r="181" spans="1:3" ht="15.5">
-      <c r="A181" t="s">
-        <v>15</v>
-      </c>
-      <c r="B181" s="5" t="s">
-        <v>114</v>
-      </c>
-      <c r="C181">
-        <v>120775</v>
-      </c>
-    </row>
-    <row r="182" spans="1:3" ht="15.5">
-      <c r="A182" t="s">
-        <v>15</v>
-      </c>
-      <c r="B182" s="5" t="s">
-        <v>115</v>
-      </c>
-      <c r="C182">
-        <v>120775</v>
-      </c>
-    </row>
-    <row r="183" spans="1:3" ht="15.5">
-      <c r="A183" t="s">
-        <v>15</v>
-      </c>
-      <c r="B183" s="5" t="s">
-        <v>116</v>
-      </c>
-      <c r="C183">
-        <v>120775</v>
-      </c>
-    </row>
-    <row r="184" spans="1:3" ht="15.5">
-      <c r="A184" t="s">
-        <v>15</v>
-      </c>
-      <c r="B184" s="5" t="s">
-        <v>117</v>
-      </c>
-      <c r="C184">
-        <v>120775</v>
-      </c>
-    </row>
-    <row r="185" spans="1:3" ht="15.5">
-      <c r="A185" t="s">
-        <v>15</v>
-      </c>
-      <c r="B185" s="5" t="s">
-        <v>118</v>
-      </c>
-      <c r="C185">
-        <v>120775</v>
-      </c>
-    </row>
-    <row r="186" spans="1:3" ht="15.5">
-      <c r="A186" t="s">
-        <v>15</v>
-      </c>
-      <c r="B186" s="5" t="s">
-        <v>119</v>
-      </c>
-      <c r="C186">
-        <v>120775</v>
-      </c>
-    </row>
-    <row r="187" spans="1:3" ht="15.5">
-      <c r="A187" t="s">
-        <v>15</v>
-      </c>
-      <c r="B187" s="5" t="s">
-        <v>120</v>
-      </c>
-      <c r="C187">
-        <v>120775</v>
-      </c>
-    </row>
-    <row r="188" spans="1:3" ht="15.5">
-      <c r="A188" t="s">
-        <v>15</v>
-      </c>
-      <c r="B188" s="5" t="s">
-        <v>121</v>
-      </c>
-      <c r="C188">
-        <v>120775</v>
-      </c>
-    </row>
-    <row r="189" spans="1:3" ht="15.5">
-      <c r="A189" t="s">
-        <v>15</v>
-      </c>
-      <c r="B189" s="5" t="s">
-        <v>122</v>
-      </c>
-      <c r="C189">
-        <v>120775</v>
-      </c>
-    </row>
-    <row r="190" spans="1:3" ht="15.5">
-      <c r="A190" t="s">
-        <v>15</v>
-      </c>
-      <c r="B190" s="5" t="s">
-        <v>123</v>
-      </c>
-      <c r="C190">
-        <v>120775</v>
-      </c>
-    </row>
-    <row r="191" spans="1:3" ht="15.5">
-      <c r="A191" t="s">
-        <v>15</v>
-      </c>
-      <c r="B191" s="5" t="s">
-        <v>124</v>
-      </c>
-      <c r="C191">
-        <v>120775</v>
-      </c>
-    </row>
-    <row r="192" spans="1:3" ht="15.5">
-      <c r="A192" t="s">
-        <v>15</v>
-      </c>
-      <c r="B192" s="5" t="s">
-        <v>125</v>
-      </c>
-      <c r="C192">
-        <v>120775</v>
-      </c>
-    </row>
-    <row r="193" spans="1:3" ht="15.5">
-      <c r="A193" t="s">
-        <v>15</v>
-      </c>
-      <c r="B193" s="5" t="s">
-        <v>126</v>
-      </c>
-      <c r="C193">
-        <v>120775</v>
-      </c>
-    </row>
-    <row r="194" spans="1:3" ht="15.5">
-      <c r="A194" t="s">
-        <v>15</v>
-      </c>
-      <c r="B194" s="5" t="s">
-        <v>127</v>
-      </c>
-      <c r="C194">
-        <v>120775</v>
-      </c>
-    </row>
-    <row r="195" spans="1:3" ht="15.5">
-      <c r="A195" t="s">
-        <v>15</v>
-      </c>
-      <c r="B195" s="5" t="s">
-        <v>128</v>
-      </c>
-      <c r="C195">
-        <v>120775</v>
-      </c>
-    </row>
-    <row r="196" spans="1:3" ht="15.5">
-      <c r="A196" t="s">
-        <v>15</v>
-      </c>
-      <c r="B196" s="5" t="s">
-        <v>129</v>
-      </c>
-      <c r="C196">
-        <v>120775</v>
-      </c>
-    </row>
-    <row r="197" spans="1:3" ht="15.5">
-      <c r="A197" t="s">
-        <v>15</v>
-      </c>
-      <c r="B197" s="5" t="s">
-        <v>130</v>
-      </c>
-      <c r="C197">
-        <v>120775</v>
-      </c>
-    </row>
-    <row r="198" spans="1:3" ht="15.5">
-      <c r="A198" t="s">
-        <v>15</v>
-      </c>
-      <c r="B198" s="5" t="s">
-        <v>131</v>
-      </c>
-      <c r="C198">
-        <v>120775</v>
-      </c>
-    </row>
-    <row r="199" spans="1:3" ht="15.5">
-      <c r="A199" t="s">
-        <v>15</v>
-      </c>
-      <c r="B199" s="5" t="s">
-        <v>132</v>
-      </c>
-      <c r="C199">
-        <v>120775</v>
-      </c>
-    </row>
-    <row r="200" spans="1:3" ht="15.5">
-      <c r="A200" t="s">
-        <v>15</v>
-      </c>
-      <c r="B200" s="5" t="s">
-        <v>133</v>
-      </c>
-      <c r="C200">
-        <v>120775</v>
-      </c>
-    </row>
-    <row r="201" spans="1:3" ht="15.5">
-      <c r="A201" t="s">
-        <v>15</v>
-      </c>
-      <c r="B201" s="5" t="s">
-        <v>134</v>
-      </c>
-      <c r="C201">
-        <v>120775</v>
-      </c>
-    </row>
-    <row r="202" spans="1:3" ht="15.5">
-      <c r="A202" t="s">
-        <v>15</v>
-      </c>
-      <c r="B202" s="5" t="s">
-        <v>135</v>
-      </c>
-      <c r="C202">
-        <v>120775</v>
-      </c>
-    </row>
-    <row r="203" spans="1:3" ht="15.5">
-      <c r="A203" t="s">
-        <v>15</v>
-      </c>
-      <c r="B203" s="5" t="s">
-        <v>136</v>
-      </c>
-      <c r="C203">
-        <v>120775</v>
-      </c>
-    </row>
-    <row r="204" spans="1:3" ht="15.5">
-      <c r="A204" t="s">
-        <v>15</v>
-      </c>
-      <c r="B204" s="5" t="s">
-        <v>137</v>
-      </c>
-      <c r="C204">
-        <v>120775</v>
-      </c>
-    </row>
-    <row r="205" spans="1:3" ht="15.5">
-      <c r="A205" t="s">
-        <v>15</v>
-      </c>
-      <c r="B205" s="5" t="s">
-        <v>138</v>
-      </c>
-      <c r="C205">
-        <v>120775</v>
-      </c>
-    </row>
-    <row r="206" spans="1:3" ht="15.5">
-      <c r="A206" t="s">
-        <v>15</v>
-      </c>
-      <c r="B206" s="5" t="s">
-        <v>139</v>
-      </c>
-      <c r="C206">
-        <v>120775</v>
-      </c>
-    </row>
-    <row r="207" spans="1:3" ht="15.5">
-      <c r="A207" t="s">
-        <v>15</v>
-      </c>
-      <c r="B207" s="5" t="s">
-        <v>140</v>
-      </c>
-      <c r="C207">
-        <v>120775</v>
-      </c>
-    </row>
-    <row r="208" spans="1:3" ht="15.5">
-      <c r="A208" t="s">
-        <v>15</v>
-      </c>
-      <c r="B208" s="5" t="s">
-        <v>141</v>
-      </c>
-      <c r="C208">
-        <v>120775</v>
-      </c>
-    </row>
-    <row r="209" spans="1:3" ht="15.5">
-      <c r="A209" t="s">
-        <v>15</v>
-      </c>
-      <c r="B209" s="5" t="s">
-        <v>142</v>
-      </c>
-      <c r="C209">
-        <v>120775</v>
-      </c>
-    </row>
-    <row r="210" spans="1:3" ht="15.5">
-      <c r="A210" t="s">
-        <v>15</v>
-      </c>
-      <c r="B210" s="5" t="s">
-        <v>143</v>
-      </c>
-      <c r="C210">
-        <v>120775</v>
-      </c>
-    </row>
-    <row r="211" spans="1:3" ht="15.5">
-      <c r="A211" t="s">
-        <v>15</v>
-      </c>
-      <c r="B211" s="5" t="s">
-        <v>144</v>
-      </c>
-      <c r="C211">
-        <v>120775</v>
-      </c>
-    </row>
-    <row r="212" spans="1:3" ht="15.5">
-      <c r="A212" t="s">
-        <v>15</v>
-      </c>
-      <c r="B212" s="5" t="s">
-        <v>145</v>
-      </c>
-      <c r="C212">
-        <v>120775</v>
-      </c>
-    </row>
-    <row r="213" spans="1:3" ht="15.5">
-      <c r="A213" t="s">
-        <v>15</v>
-      </c>
-      <c r="B213" s="5" t="s">
-        <v>146</v>
-      </c>
-      <c r="C213">
-        <v>120775</v>
-      </c>
-    </row>
-    <row r="214" spans="1:3" ht="15.5">
-      <c r="A214" t="s">
-        <v>15</v>
-      </c>
-      <c r="B214" s="5" t="s">
-        <v>147</v>
-      </c>
-      <c r="C214">
-        <v>120775</v>
-      </c>
-    </row>
-    <row r="215" spans="1:3" ht="15.5">
-      <c r="A215" t="s">
-        <v>15</v>
-      </c>
-      <c r="B215" s="5" t="s">
-        <v>148</v>
-      </c>
-      <c r="C215">
-        <v>120775</v>
-      </c>
-    </row>
-    <row r="216" spans="1:3" ht="15.5">
-      <c r="A216" t="s">
-        <v>15</v>
-      </c>
-      <c r="B216" s="5" t="s">
-        <v>149</v>
-      </c>
-      <c r="C216">
-        <v>120775</v>
-      </c>
-    </row>
-    <row r="217" spans="1:3" ht="15.5">
-      <c r="A217" t="s">
-        <v>15</v>
-      </c>
-      <c r="B217" s="5" t="s">
-        <v>150</v>
-      </c>
-      <c r="C217">
-        <v>120775</v>
-      </c>
-    </row>
-    <row r="218" spans="1:3" ht="15.5">
-      <c r="A218" t="s">
-        <v>15</v>
-      </c>
-      <c r="B218" s="5" t="s">
-        <v>151</v>
-      </c>
-      <c r="C218">
-        <v>120775</v>
-      </c>
-    </row>
-    <row r="219" spans="1:3" ht="15.5">
-      <c r="A219" t="s">
-        <v>15</v>
-      </c>
-      <c r="B219" s="5" t="s">
-        <v>152</v>
-      </c>
-      <c r="C219">
-        <v>120775</v>
-      </c>
-    </row>
-    <row r="220" spans="1:3" ht="15.5">
-      <c r="A220" t="s">
-        <v>15</v>
-      </c>
-      <c r="B220" s="5" t="s">
-        <v>153</v>
-      </c>
-      <c r="C220">
-        <v>120775</v>
-      </c>
-    </row>
-    <row r="221" spans="1:3" ht="15.5">
-      <c r="A221" t="s">
-        <v>15</v>
-      </c>
-      <c r="B221" s="5" t="s">
-        <v>154</v>
-      </c>
-      <c r="C221">
-        <v>120775</v>
-      </c>
-    </row>
-    <row r="222" spans="1:3" ht="15.5">
-      <c r="A222" t="s">
-        <v>15</v>
-      </c>
-      <c r="B222" s="5" t="s">
-        <v>155</v>
-      </c>
-      <c r="C222">
-        <v>120775</v>
-      </c>
-    </row>
-    <row r="223" spans="1:3" ht="15.5">
-      <c r="A223" t="s">
-        <v>15</v>
-      </c>
-      <c r="B223" s="5" t="s">
-        <v>156</v>
-      </c>
-      <c r="C223">
-        <v>120775</v>
-      </c>
-    </row>
-    <row r="224" spans="1:3" ht="15.5">
-      <c r="A224" t="s">
-        <v>15</v>
-      </c>
-      <c r="B224" s="5" t="s">
-        <v>157</v>
-      </c>
-      <c r="C224">
-        <v>120775</v>
-      </c>
-    </row>
-    <row r="225" spans="1:3" ht="15.5">
-      <c r="A225" t="s">
-        <v>15</v>
-      </c>
-      <c r="B225" s="5" t="s">
-        <v>158</v>
-      </c>
-      <c r="C225">
-        <v>120775</v>
-      </c>
-    </row>
-    <row r="226" spans="1:3" ht="15.5">
-      <c r="A226" t="s">
-        <v>15</v>
-      </c>
-      <c r="B226" s="5" t="s">
-        <v>159</v>
-      </c>
-      <c r="C226">
-        <v>120775</v>
-      </c>
-    </row>
-    <row r="227" spans="1:3" ht="15.5">
-      <c r="A227" t="s">
-        <v>15</v>
-      </c>
-      <c r="B227" s="5" t="s">
-        <v>160</v>
-      </c>
-      <c r="C227">
-        <v>120775</v>
-      </c>
-    </row>
-    <row r="228" spans="1:3" ht="15.5">
-      <c r="A228" t="s">
-        <v>15</v>
-      </c>
-      <c r="B228" s="5" t="s">
-        <v>161</v>
-      </c>
-      <c r="C228">
-        <v>120775</v>
-      </c>
-    </row>
-    <row r="229" spans="1:3" ht="15.5">
-      <c r="A229" t="s">
-        <v>15</v>
-      </c>
-      <c r="B229" s="5" t="s">
-        <v>162</v>
-      </c>
-      <c r="C229">
-        <v>120775</v>
-      </c>
-    </row>
-    <row r="230" spans="1:3" ht="15.5">
-      <c r="A230" t="s">
-        <v>15</v>
-      </c>
-      <c r="B230" s="5" t="s">
-        <v>163</v>
-      </c>
-      <c r="C230">
-        <v>120775</v>
-      </c>
-    </row>
-    <row r="231" spans="1:3" ht="15.5">
-      <c r="A231" t="s">
-        <v>15</v>
-      </c>
-      <c r="B231" s="5" t="s">
-        <v>164</v>
-      </c>
-      <c r="C231">
-        <v>120775</v>
-      </c>
-    </row>
-    <row r="232" spans="1:3" ht="15.5">
-      <c r="A232" t="s">
-        <v>15</v>
-      </c>
-      <c r="B232" s="5" t="s">
-        <v>165</v>
-      </c>
-      <c r="C232">
-        <v>120775</v>
-      </c>
-    </row>
-    <row r="233" spans="1:3" ht="15.5">
-      <c r="A233" t="s">
-        <v>15</v>
-      </c>
-      <c r="B233" s="5" t="s">
-        <v>166</v>
-      </c>
-      <c r="C233">
-        <v>120775</v>
-      </c>
-    </row>
-    <row r="234" spans="1:3" ht="15.5">
-      <c r="A234" t="s">
-        <v>15</v>
-      </c>
-      <c r="B234" s="5" t="s">
-        <v>167</v>
-      </c>
-      <c r="C234">
-        <v>120775</v>
-      </c>
-    </row>
-    <row r="235" spans="1:3" ht="15.5">
-      <c r="A235" t="s">
-        <v>15</v>
-      </c>
-      <c r="B235" s="5" t="s">
-        <v>168</v>
-      </c>
-      <c r="C235">
-        <v>120775</v>
-      </c>
-    </row>
-    <row r="236" spans="1:3" ht="15.5">
-      <c r="A236" t="s">
-        <v>15</v>
-      </c>
-      <c r="B236" s="5" t="s">
-        <v>169</v>
-      </c>
-      <c r="C236">
-        <v>120775</v>
-      </c>
-    </row>
-    <row r="237" spans="1:3" ht="15.5">
-      <c r="A237" t="s">
-        <v>15</v>
-      </c>
-      <c r="B237" s="5" t="s">
-        <v>170</v>
-      </c>
-      <c r="C237">
-        <v>120775</v>
-      </c>
-    </row>
-    <row r="238" spans="1:3" ht="15.5">
-      <c r="A238" t="s">
-        <v>15</v>
-      </c>
-      <c r="B238" s="5" t="s">
-        <v>171</v>
-      </c>
-      <c r="C238">
-        <v>120775</v>
-      </c>
-    </row>
-    <row r="239" spans="1:3" ht="15.5">
-      <c r="A239" t="s">
-        <v>15</v>
-      </c>
-      <c r="B239" s="5" t="s">
-        <v>172</v>
-      </c>
-      <c r="C239">
-        <v>120775</v>
-      </c>
-    </row>
-    <row r="240" spans="1:3" ht="15.5">
-      <c r="A240" t="s">
-        <v>15</v>
-      </c>
-      <c r="B240" s="5" t="s">
-        <v>173</v>
-      </c>
-      <c r="C240">
-        <v>120775</v>
-      </c>
-    </row>
-    <row r="241" spans="1:3" ht="15.5">
-      <c r="A241" t="s">
-        <v>15</v>
-      </c>
-      <c r="B241" s="5" t="s">
-        <v>174</v>
-      </c>
-      <c r="C241">
-        <v>120775</v>
-      </c>
-    </row>
-  </sheetData>
-  <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2:A241" xr:uid="{E84901F5-638B-4BA2-A0B3-802A5C8E717B}">
-      <formula1>"HAIL_TESTER, MLT_TESTER, THERMAL_CYCLING, DAMP_HEAT, PCT, COMMON_PARTS"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -6685,15 +4182,15 @@
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E0E37CA3-E383-451B-A722-9F0EA8A56E91}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
     <ds:schemaRef ds:uri="32f52b41-3b94-4090-a175-52d6bdf443eb"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
📊 Update Excel files from OneDrive - 2025-09-16 10:40:51
</commit_message>
<xml_diff>
--- a/backend/data/Spare_Parts_Inventory.xlsx
+++ b/backend/data/Spare_Parts_Inventory.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://vikramsolar0-my.sharepoint.com/personal/naveen_chamaria_vikramsolar_com/Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="426" documentId="8_{319E19CD-5EDD-431C-9D80-979664711085}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{26D211E6-1DBD-4EDE-A0F2-4FE7CCC2ED50}"/>
+  <xr:revisionPtr revIDLastSave="428" documentId="8_{319E19CD-5EDD-431C-9D80-979664711085}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0EB74042-E6C6-46C8-B3D9-828FE03E59EB}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{72449171-FCEF-49D6-AEAC-5AACDA2C6B26}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="692" uniqueCount="282">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="694" uniqueCount="283">
   <si>
     <t>Equipment_Category</t>
   </si>
@@ -883,6 +883,9 @@
   </si>
   <si>
     <t>holder</t>
+  </si>
+  <si>
+    <t>Inactive</t>
   </si>
 </sst>
 </file>
@@ -1294,8 +1297,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{94C1C842-7533-49D8-BD7E-9BF474738299}">
   <dimension ref="A1:L335"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="82" workbookViewId="0">
-      <selection activeCell="G342" sqref="G342"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="82" workbookViewId="0">
+      <selection activeCell="L5" sqref="L5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -1364,6 +1367,9 @@
       <c r="F2">
         <v>0</v>
       </c>
+      <c r="L2" t="s">
+        <v>282</v>
+      </c>
     </row>
     <row r="3" spans="1:12">
       <c r="A3" t="s">
@@ -1377,6 +1383,9 @@
       </c>
       <c r="F3">
         <v>0</v>
+      </c>
+      <c r="L3" t="s">
+        <v>282</v>
       </c>
     </row>
     <row r="4" spans="1:12">

</xml_diff>